<commit_message>
CCRU KPI templates fix
</commit_message>
<xml_diff>
--- a/Projects/CCRU/Data/KPIs_2019/PoS 2019 - IC HoReCa BarTavernClub.xlsx
+++ b/Projects/CCRU/Data/KPIs_2019/PoS 2019 - IC HoReCa BarTavernClub.xlsx
@@ -8,10 +8,10 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\My folder\RED\POS\POS_2019-10-17\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ABA6E3A4-6212-408B-B499-6E0411E179F1}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D847F34E-07A2-45F7-99A3-BC4705E0D651}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <workbookProtection lockWindows="1"/>
   <bookViews>
-    <workbookView xWindow="384" yWindow="384" windowWidth="17280" windowHeight="9024" tabRatio="587" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="587" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="HoReCa Bar Tavern_Night Club" sheetId="1" r:id="rId1"/>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="479" uniqueCount="186">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="478" uniqueCount="184">
   <si>
     <t>Sorting</t>
   </si>
@@ -493,12 +493,6 @@
   </si>
   <si>
     <t>Импульс: Дисплей</t>
-  </si>
-  <si>
-    <t>Brand: Schweppes, Coca-Cola, Burn</t>
-  </si>
-  <si>
-    <t>Schweppes, Coca-Cola, Burn</t>
   </si>
   <si>
     <t>Glass, glass, GLASS, Can, CAN, can</t>
@@ -679,12 +673,18 @@
       <charset val="1"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF92D050"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="4">
@@ -742,7 +742,7 @@
     <xf numFmtId="164" fontId="5" fillId="0" borderId="0" applyBorder="0" applyProtection="0"/>
     <xf numFmtId="9" fontId="5" fillId="0" borderId="0" applyBorder="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="23">
+  <cellXfs count="25">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -808,6 +808,12 @@
     </xf>
     <xf numFmtId="49" fontId="4" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
@@ -1196,8 +1202,8 @@
   <dimension ref="A1:AMK39"/>
   <sheetViews>
     <sheetView windowProtection="1" tabSelected="1" zoomScale="65" zoomScaleNormal="65" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="AA32" sqref="AA32"/>
+      <pane ySplit="1" topLeftCell="A17" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="M30" sqref="M30:N30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.25"/>
@@ -3370,7 +3376,7 @@
         <v>141</v>
       </c>
       <c r="AA28" s="7" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
       <c r="AB28" s="7"/>
       <c r="AC28" s="7"/>
@@ -3445,7 +3451,7 @@
         <v>141</v>
       </c>
       <c r="AA29" s="7" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
       <c r="AB29" s="7"/>
       <c r="AC29" s="7"/>
@@ -3503,27 +3509,25 @@
       </c>
       <c r="K30" s="7"/>
       <c r="L30" s="7"/>
-      <c r="M30" s="7" t="s">
-        <v>147</v>
-      </c>
-      <c r="N30" s="21" t="s">
-        <v>148</v>
+      <c r="M30" s="23" t="s">
+        <v>124</v>
+      </c>
+      <c r="N30" s="24" t="s">
+        <v>125</v>
       </c>
       <c r="O30" s="7"/>
       <c r="P30" s="7"/>
       <c r="Q30" s="7"/>
-      <c r="R30" s="21" t="s">
-        <v>148</v>
-      </c>
+      <c r="R30" s="21"/>
       <c r="S30" s="7" t="s">
         <v>54</v>
       </c>
-      <c r="T30" s="7" t="s">
-        <v>140</v>
+      <c r="T30" s="23" t="s">
+        <v>126</v>
       </c>
       <c r="U30" s="7"/>
       <c r="V30" s="7" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="W30" s="7"/>
       <c r="X30" s="7"/>
@@ -3532,7 +3536,7 @@
         <v>141</v>
       </c>
       <c r="AA30" s="7" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
       <c r="AB30" s="7"/>
       <c r="AC30" s="7"/>
@@ -3572,10 +3576,10 @@
         <v>142</v>
       </c>
       <c r="F31" s="7" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="G31" s="7" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="H31" s="7" t="s">
         <v>113</v>
@@ -3605,7 +3609,7 @@
         <v>141</v>
       </c>
       <c r="AA31" s="7" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
       <c r="AB31" s="7"/>
       <c r="AC31" s="7"/>
@@ -3626,7 +3630,7 @@
         <v>25</v>
       </c>
       <c r="AL31" s="12" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="AM31" s="7">
         <v>400</v>
@@ -3649,10 +3653,10 @@
         <v>142</v>
       </c>
       <c r="F32" s="7" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="G32" s="7" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="H32" s="7" t="s">
         <v>53</v>
@@ -3664,13 +3668,13 @@
       <c r="K32" s="7"/>
       <c r="L32" s="7"/>
       <c r="M32" s="7" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="N32" s="7" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="O32" s="7" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="P32" s="7"/>
       <c r="Q32" s="7"/>
@@ -3679,7 +3683,7 @@
         <v>54</v>
       </c>
       <c r="T32" s="7" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="U32" s="7"/>
       <c r="V32" s="7"/>
@@ -3690,7 +3694,7 @@
         <v>141</v>
       </c>
       <c r="AA32" s="7" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
       <c r="AB32" s="7"/>
       <c r="AC32" s="7"/>
@@ -3724,22 +3728,22 @@
         <v>40</v>
       </c>
       <c r="D33" s="7" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="E33" s="19" t="s">
         <v>110</v>
       </c>
       <c r="F33" s="19" t="s">
+        <v>156</v>
+      </c>
+      <c r="G33" s="19" t="s">
+        <v>157</v>
+      </c>
+      <c r="H33" s="7" t="s">
         <v>158</v>
       </c>
-      <c r="G33" s="19" t="s">
+      <c r="I33" s="7" t="s">
         <v>159</v>
-      </c>
-      <c r="H33" s="7" t="s">
-        <v>160</v>
-      </c>
-      <c r="I33" s="7" t="s">
-        <v>161</v>
       </c>
       <c r="J33" s="7"/>
       <c r="K33" s="7"/>
@@ -3752,7 +3756,7 @@
       <c r="R33" s="7"/>
       <c r="S33" s="7"/>
       <c r="T33" s="7" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="U33" s="7"/>
       <c r="V33" s="7"/>
@@ -3774,7 +3778,7 @@
         <v>38</v>
       </c>
       <c r="AL33" s="12" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="AM33" s="7"/>
     </row>
@@ -3789,29 +3793,29 @@
         <v>40</v>
       </c>
       <c r="D34" s="7" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="E34" s="19" t="s">
         <v>135</v>
       </c>
       <c r="F34" s="19" t="s">
+        <v>162</v>
+      </c>
+      <c r="G34" s="19" t="s">
+        <v>163</v>
+      </c>
+      <c r="H34" s="7" t="s">
         <v>164</v>
       </c>
-      <c r="G34" s="19" t="s">
+      <c r="I34" s="7" t="s">
         <v>165</v>
-      </c>
-      <c r="H34" s="7" t="s">
-        <v>166</v>
-      </c>
-      <c r="I34" s="7" t="s">
-        <v>167</v>
       </c>
       <c r="J34" s="7"/>
       <c r="K34" s="7"/>
       <c r="L34" s="7"/>
       <c r="M34" s="7"/>
       <c r="N34" s="12" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="O34" s="7"/>
       <c r="P34" s="7"/>
@@ -3819,7 +3823,7 @@
       <c r="R34" s="7"/>
       <c r="S34" s="7"/>
       <c r="T34" s="7" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="U34" s="7"/>
       <c r="V34" s="7"/>
@@ -3856,29 +3860,29 @@
         <v>40</v>
       </c>
       <c r="D35" s="7" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="E35" s="7" t="s">
         <v>142</v>
       </c>
       <c r="F35" s="7" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="G35" s="7" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="H35" s="7" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="I35" s="7" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="J35" s="7"/>
       <c r="K35" s="7"/>
       <c r="L35" s="7"/>
       <c r="M35" s="7"/>
       <c r="N35" s="12" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
       <c r="O35" s="7"/>
       <c r="P35" s="7"/>
@@ -3886,7 +3890,7 @@
       <c r="R35" s="7"/>
       <c r="S35" s="7"/>
       <c r="T35" s="7" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="U35" s="7"/>
       <c r="V35" s="7"/>
@@ -3923,29 +3927,29 @@
         <v>40</v>
       </c>
       <c r="D36" s="7" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="E36" s="7" t="s">
         <v>142</v>
       </c>
       <c r="F36" s="7" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="G36" s="7" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="H36" s="7" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="I36" s="7" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="J36" s="7"/>
       <c r="K36" s="7"/>
       <c r="L36" s="7"/>
       <c r="M36" s="7"/>
       <c r="N36" s="12" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="O36" s="7"/>
       <c r="P36" s="7"/>
@@ -3953,7 +3957,7 @@
       <c r="R36" s="7"/>
       <c r="S36" s="7"/>
       <c r="T36" s="7" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="U36" s="7"/>
       <c r="V36" s="7"/>
@@ -3990,31 +3994,31 @@
         <v>40</v>
       </c>
       <c r="D37" s="7" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="E37" s="7" t="s">
+        <v>171</v>
+      </c>
+      <c r="F37" s="19" t="s">
+        <v>172</v>
+      </c>
+      <c r="G37" s="19" t="s">
         <v>173</v>
       </c>
-      <c r="F37" s="19" t="s">
-        <v>174</v>
-      </c>
-      <c r="G37" s="19" t="s">
-        <v>175</v>
-      </c>
       <c r="H37" s="7" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="I37" s="7" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="J37" s="7"/>
       <c r="K37" s="7"/>
       <c r="L37" s="7"/>
       <c r="M37" s="7" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="N37" s="12" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="O37" s="7"/>
       <c r="P37" s="7"/>
@@ -4022,7 +4026,7 @@
       <c r="R37" s="7"/>
       <c r="S37" s="7"/>
       <c r="T37" s="7" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="U37" s="7"/>
       <c r="V37" s="7"/>
@@ -4044,7 +4048,7 @@
         <v>44</v>
       </c>
       <c r="AL37" s="12" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="AM37" s="7"/>
     </row>
@@ -4059,31 +4063,31 @@
         <v>40</v>
       </c>
       <c r="D38" s="7" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="E38" s="7" t="s">
+        <v>171</v>
+      </c>
+      <c r="F38" s="19" t="s">
+        <v>172</v>
+      </c>
+      <c r="G38" s="19" t="s">
         <v>173</v>
       </c>
-      <c r="F38" s="19" t="s">
-        <v>174</v>
-      </c>
-      <c r="G38" s="19" t="s">
-        <v>175</v>
-      </c>
       <c r="H38" s="7" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="I38" s="7" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="J38" s="7"/>
       <c r="K38" s="7"/>
       <c r="L38" s="7"/>
       <c r="M38" s="7" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="N38" s="12" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="O38" s="7"/>
       <c r="P38" s="7"/>
@@ -4091,7 +4095,7 @@
       <c r="R38" s="7"/>
       <c r="S38" s="7"/>
       <c r="T38" s="7" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="U38" s="7"/>
       <c r="V38" s="7"/>
@@ -4113,7 +4117,7 @@
         <v>45</v>
       </c>
       <c r="AL38" s="12" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="AM38" s="7"/>
     </row>
@@ -4128,20 +4132,20 @@
         <v>40</v>
       </c>
       <c r="D39" s="7" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="E39" s="19"/>
       <c r="F39" s="19" t="s">
+        <v>178</v>
+      </c>
+      <c r="G39" s="19" t="s">
+        <v>179</v>
+      </c>
+      <c r="H39" s="7" t="s">
+        <v>179</v>
+      </c>
+      <c r="I39" s="7" t="s">
         <v>180</v>
-      </c>
-      <c r="G39" s="19" t="s">
-        <v>181</v>
-      </c>
-      <c r="H39" s="7" t="s">
-        <v>181</v>
-      </c>
-      <c r="I39" s="7" t="s">
-        <v>182</v>
       </c>
       <c r="J39" s="15"/>
       <c r="K39" s="15"/>
@@ -4154,7 +4158,7 @@
       <c r="R39" s="7"/>
       <c r="S39" s="7"/>
       <c r="T39" s="7" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="U39" s="7"/>
       <c r="V39" s="7"/>

</xml_diff>

<commit_message>
PROS-13425 - CCRU - KPI calculation fix
</commit_message>
<xml_diff>
--- a/Projects/CCRU/Data/KPIs_2019/PoS 2019 - IC HoReCa BarTavernClub.xlsx
+++ b/Projects/CCRU/Data/KPIs_2019/PoS 2019 - IC HoReCa BarTavernClub.xlsx
@@ -1,33 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21328"/>
-  <workbookPr defaultThemeVersion="166925"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\My folder\RED\POS 2019\POS_2019-12-16\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{32562A94-DCE6-4D39-8829-1DE2E44499C4}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
-  <workbookProtection lockWindows="1"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="Calc"/>
+  <workbookPr backupFile="false" showObjects="all" date1904="false"/>
+  <workbookProtection/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="730" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="993" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
-    <sheet name="HoReCa Bar Tavern_Night Club" sheetId="1" r:id="rId1"/>
+    <sheet name="HoReCa Bar Tavern_Night Club" sheetId="1" state="visible" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0">'HoReCa Bar Tavern_Night Club'!$A$1:$AO$39</definedName>
-    <definedName name="_FilterDatabase_0" localSheetId="0">'HoReCa Bar Tavern_Night Club'!$A$1:$AO$39</definedName>
+    <definedName function="false" hidden="true" localSheetId="0" name="_xlnm._FilterDatabase" vbProcedure="false">'HoReCa Bar Tavern_Night Club'!$A$1:$AO$39</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_FilterDatabase_0" vbProcedure="false">'HoReCa Bar Tavern_Night Club'!$A$1:$AO$39</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase" vbProcedure="false">'HoReCa Bar Tavern_Night Club'!$A$1:$AO$39</definedName>
   </definedNames>
-  <calcPr calcId="191029" iterateDelta="1E-4"/>
+  <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
   <extLst>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-      </xcalcf:calcFeatures>
-    </ext>
     <ext xmlns:loext="http://schemas.libreoffice.org/" uri="{7626C862-2A13-11E5-B345-FEFF819CDC9F}">
       <loext:extCalcPr stringRefSyntax="ExcelA1"/>
     </ext>
@@ -38,142 +27,142 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="482" uniqueCount="189">
   <si>
-    <t>Sorting</t>
-  </si>
-  <si>
-    <t>SAP PoS</t>
-  </si>
-  <si>
-    <t>Channel</t>
-  </si>
-  <si>
-    <t>KPI Type</t>
-  </si>
-  <si>
-    <t>SAP KPI</t>
-  </si>
-  <si>
-    <t>KPI name Eng</t>
-  </si>
-  <si>
-    <t>KPI name Rus</t>
-  </si>
-  <si>
-    <t>Formula</t>
-  </si>
-  <si>
-    <t>Category KPI Type</t>
-  </si>
-  <si>
-    <t>Category KPI Value</t>
-  </si>
-  <si>
-    <t>Result Format</t>
-  </si>
-  <si>
-    <t>Target</t>
-  </si>
-  <si>
-    <t>target_min</t>
-  </si>
-  <si>
-    <t>target_max</t>
-  </si>
-  <si>
-    <t>SKU</t>
-  </si>
-  <si>
-    <t>Values</t>
-  </si>
-  <si>
-    <t>Product Category</t>
-  </si>
-  <si>
-    <t>Manufacturer</t>
-  </si>
-  <si>
-    <t>Sub category</t>
-  </si>
-  <si>
-    <t>Brand</t>
-  </si>
-  <si>
-    <t>Logical Operator</t>
-  </si>
-  <si>
-    <t>Type</t>
-  </si>
-  <si>
-    <t>Size</t>
-  </si>
-  <si>
-    <t>Form Factor</t>
-  </si>
-  <si>
-    <t>Products to exclude</t>
-  </si>
-  <si>
-    <t>Zone to include</t>
-  </si>
-  <si>
-    <t>Locations to exclude</t>
-  </si>
-  <si>
-    <t>Locations to include</t>
-  </si>
-  <si>
-    <t>Scenes to include</t>
-  </si>
-  <si>
-    <t>Scenes to exclude</t>
-  </si>
-  <si>
-    <t>sub locations to include</t>
-  </si>
-  <si>
-    <t>sub locations to exclude</t>
-  </si>
-  <si>
-    <t>score_func</t>
-  </si>
-  <si>
-    <t>KPI Weight</t>
-  </si>
-  <si>
-    <t>score_min</t>
-  </si>
-  <si>
-    <t>score_max</t>
-  </si>
-  <si>
-    <t>Comments</t>
-  </si>
-  <si>
-    <t>level</t>
-  </si>
-  <si>
-    <t>KPI ID</t>
-  </si>
-  <si>
-    <t>Children</t>
-  </si>
-  <si>
-    <t>Parent</t>
-  </si>
-  <si>
-    <t>RD38000023</t>
-  </si>
-  <si>
-    <t>HoReCa_Bar_Tavern_Night_Clubs</t>
-  </si>
-  <si>
-    <t>Group</t>
-  </si>
-  <si>
-    <t>Availability</t>
-  </si>
-  <si>
-    <t>Представленность</t>
+    <t xml:space="preserve">Sorting</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SAP PoS</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Channel</t>
+  </si>
+  <si>
+    <t xml:space="preserve">KPI Type</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SAP KPI</t>
+  </si>
+  <si>
+    <t xml:space="preserve">KPI name Eng</t>
+  </si>
+  <si>
+    <t xml:space="preserve">KPI name Rus</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Formula</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Category KPI Type</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Category KPI Value</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Result Format</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Target</t>
+  </si>
+  <si>
+    <t xml:space="preserve">target_min</t>
+  </si>
+  <si>
+    <t xml:space="preserve">target_max</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SKU</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Values</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Product Category</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Manufacturer</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Sub category</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Brand</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Logical Operator</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Type</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Size</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Form Factor</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Products to exclude</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Zone to include</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Locations to exclude</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Locations to include</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Scenes to include</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Scenes to exclude</t>
+  </si>
+  <si>
+    <t xml:space="preserve">sub locations to include</t>
+  </si>
+  <si>
+    <t xml:space="preserve">sub locations to exclude</t>
+  </si>
+  <si>
+    <t xml:space="preserve">score_func</t>
+  </si>
+  <si>
+    <t xml:space="preserve">KPI Weight</t>
+  </si>
+  <si>
+    <t xml:space="preserve">score_min</t>
+  </si>
+  <si>
+    <t xml:space="preserve">score_max</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Comments</t>
+  </si>
+  <si>
+    <t xml:space="preserve">level</t>
+  </si>
+  <si>
+    <t xml:space="preserve">KPI ID</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Children</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Parent</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RD38000023</t>
+  </si>
+  <si>
+    <t xml:space="preserve">HoReCa_Bar_Tavern_Night_Clubs</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Group</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Availability</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Представленность</t>
   </si>
   <si>
     <t xml:space="preserve">1
@@ -183,19 +172,19 @@
 </t>
   </si>
   <si>
-    <t>STANDARD 1</t>
-  </si>
-  <si>
-    <t>SSD Availability</t>
-  </si>
-  <si>
-    <t>Представленность SSD</t>
-  </si>
-  <si>
-    <t>Weighted Average</t>
-  </si>
-  <si>
-    <t>SSD</t>
+    <t xml:space="preserve">STANDARD 1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SSD Availability</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Представленность SSD</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Weighted Average</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SSD</t>
   </si>
   <si>
     <t xml:space="preserve">Weighted Average </t>
@@ -209,114 +198,117 @@
 </t>
   </si>
   <si>
-    <t>Coca-Cola - 0.33L Glass</t>
-  </si>
-  <si>
-    <t>Кока-Кола - 0.33л стекло</t>
-  </si>
-  <si>
-    <t>number of facings</t>
-  </si>
-  <si>
-    <t>OR</t>
-  </si>
-  <si>
-    <t>SKUs</t>
-  </si>
-  <si>
-    <t>Other</t>
-  </si>
-  <si>
-    <t>BINARY</t>
-  </si>
-  <si>
-    <t>Coca-Cola Zero - 0.33L Glass</t>
-  </si>
-  <si>
-    <t>Кока-Кола Зеро - 0.33л стекло</t>
-  </si>
-  <si>
-    <t>Schweppes Tonic - 0.25L Glass</t>
-  </si>
-  <si>
-    <t>Швеппс Тоник - 0.25л стекло</t>
-  </si>
-  <si>
-    <t>Schweppes Bitter Lemon - 0.25L Glass</t>
-  </si>
-  <si>
-    <t>Швеппс Биттер Лемон - 0.25л стекло</t>
-  </si>
-  <si>
-    <t>Sprite - 0.33L Glass/Fanta Orange - 0.33L Glass</t>
-  </si>
-  <si>
-    <t>Спрайт - 0.33л стекло/ Фанта Апельсин - 0.33л стекло</t>
-  </si>
-  <si>
-    <t>Sprite - 0.33L Glass, Fanta Orange - 0.33L Glass</t>
-  </si>
-  <si>
-    <t>54490970, 40822419, 87126860, 50112135</t>
-  </si>
-  <si>
-    <t>STANDARD 2</t>
-  </si>
-  <si>
-    <t>Water Availability</t>
-  </si>
-  <si>
-    <t>Представленность Воды</t>
-  </si>
-  <si>
-    <t>Water</t>
-  </si>
-  <si>
-    <t>BonAqua Still - 0.33L Glass/ BonAqua Carb - 0.33L Glass</t>
-  </si>
-  <si>
-    <t>БонАква Негаз - 0.33л стекло/БонАква Газ - 0.33л стекло</t>
-  </si>
-  <si>
-    <t>BonAqua Still - 0.33L Glass, BonAqua Carb - 0.33L Glass</t>
-  </si>
-  <si>
-    <t>90418822, 90382741</t>
-  </si>
-  <si>
-    <t>Juice (JNSD) Availability</t>
-  </si>
-  <si>
-    <t>Представленность Сока</t>
-  </si>
-  <si>
-    <t>Juices</t>
-  </si>
-  <si>
-    <t>12
+    <t xml:space="preserve">Coca-Cola - 0.33L Glass</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Кока-Кола - 0.33л стекло</t>
+  </si>
+  <si>
+    <t xml:space="preserve">number of facings</t>
+  </si>
+  <si>
+    <t xml:space="preserve">OR</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SKUs</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Other</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Panoramic Photo; SS_Panoramic Photo</t>
+  </si>
+  <si>
+    <t xml:space="preserve">BINARY</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Coca-Cola Zero - 0.33L Glass</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Кока-Кола Зеро - 0.33л стекло</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Schweppes Tonic - 0.25L Glass</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Швеппс Тоник - 0.25л стекло</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Schweppes Bitter Lemon - 0.25L Glass</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Швеппс Биттер Лемон - 0.25л стекло</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Sprite - 0.33L Glass/Fanta Orange - 0.33L Glass</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Спрайт - 0.33л стекло/ Фанта Апельсин - 0.33л стекло</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Sprite - 0.33L Glass, Fanta Orange - 0.33L Glass</t>
+  </si>
+  <si>
+    <t xml:space="preserve">54490970, 40822419, 87126860, 50112135</t>
+  </si>
+  <si>
+    <t xml:space="preserve">STANDARD 2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Water Availability</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Представленность Воды</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Water</t>
+  </si>
+  <si>
+    <t xml:space="preserve">BonAqua Still - 0.33L Glass/ BonAqua Carb - 0.33L Glass</t>
+  </si>
+  <si>
+    <t xml:space="preserve">БонАква Негаз - 0.33л стекло/БонАква Газ - 0.33л стекло</t>
+  </si>
+  <si>
+    <t xml:space="preserve">BonAqua Still - 0.33L Glass, BonAqua Carb - 0.33L Glass</t>
+  </si>
+  <si>
+    <t xml:space="preserve">90418822, 90382741</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Juice (JNSD) Availability</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Представленность Сока</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Juices</t>
+  </si>
+  <si>
+    <t xml:space="preserve">12
 13
 15</t>
   </si>
   <si>
-    <t>Rich - Apple - 0.2L Glass</t>
-  </si>
-  <si>
-    <t>Рич - Яблоко - 0.2л стекло</t>
-  </si>
-  <si>
-    <t>Rich - Orange - 0.2L Glass</t>
-  </si>
-  <si>
-    <t>Рич - Апельсин - 0.2л стекло</t>
-  </si>
-  <si>
-    <t>Rich 0.2L Glass other</t>
-  </si>
-  <si>
-    <t>Рич 0.2л стекло остальные</t>
-  </si>
-  <si>
-    <t>number of sub atomic KPI Passed</t>
+    <t xml:space="preserve">Rich - Apple - 0.2L Glass</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Рич - Яблоко - 0.2л стекло</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Rich - Orange - 0.2L Glass</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Рич - Апельсин - 0.2л стекло</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Rich 0.2L Glass other</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Рич 0.2л стекло остальные</t>
+  </si>
+  <si>
+    <t xml:space="preserve">number of sub atomic KPI Passed</t>
   </si>
   <si>
     <t xml:space="preserve">16
@@ -325,93 +317,93 @@
 </t>
   </si>
   <si>
-    <t>Rich - Peach - 0.2L Glass</t>
-  </si>
-  <si>
-    <t>Рич - Персик - 0.2л стекло</t>
-  </si>
-  <si>
-    <t>Rich - Cherry - 0.2L Glass</t>
-  </si>
-  <si>
-    <t>Рич - Вишня - 0.2л стекло</t>
-  </si>
-  <si>
-    <t>Rich - Pineapple - 0.2L Glass</t>
-  </si>
-  <si>
-    <t>Рич - Ананас - 0.2л стекло</t>
-  </si>
-  <si>
-    <t>Energy Availability</t>
-  </si>
-  <si>
-    <t>Представленность Энергетиков</t>
-  </si>
-  <si>
-    <t>Energy</t>
-  </si>
-  <si>
-    <t>767
+    <t xml:space="preserve">Rich - Peach - 0.2L Glass</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Рич - Персик - 0.2л стекло</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Rich - Cherry - 0.2L Glass</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Рич - Вишня - 0.2л стекло</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Rich - Pineapple - 0.2L Glass</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Рич - Ананас - 0.2л стекло</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Energy Availability</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Представленность Энергетиков</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Energy</t>
+  </si>
+  <si>
+    <t xml:space="preserve">767
 759</t>
   </si>
   <si>
-    <t>RD38010012</t>
-  </si>
-  <si>
-    <t>Burn Original - 0.33L</t>
-  </si>
-  <si>
-    <t>Берн Оригинальный - 0.33л</t>
-  </si>
-  <si>
-    <t>5449000148056</t>
-  </si>
-  <si>
-    <t>Burn Original - 0.5L/Burn Apple Kiwi - 0.33L</t>
-  </si>
-  <si>
-    <t>Берн Оригинальный - 0.5л/Берн Яблоко-Киви - 0.33л</t>
-  </si>
-  <si>
-    <t>Burn Original - 0.5L, Burn Apple Kiwi - 0.33L</t>
-  </si>
-  <si>
-    <t>5449000131768, 5060466510920</t>
-  </si>
-  <si>
-    <t>Coolers</t>
-  </si>
-  <si>
-    <t>Холодильники</t>
-  </si>
-  <si>
-    <t>311
+    <t xml:space="preserve">RD38010012</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Burn Original - 0.33L</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Берн Оригинальный - 0.33л</t>
+  </si>
+  <si>
+    <t xml:space="preserve">5449000148056</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Burn Original - 0.5L/Burn Apple Kiwi - 0.33L</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Берн Оригинальный - 0.5л/Берн Яблоко-Киви - 0.33л</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Burn Original - 0.5L, Burn Apple Kiwi - 0.33L</t>
+  </si>
+  <si>
+    <t xml:space="preserve">5449000131768, 5060466510920</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Coolers</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Холодильники</t>
+  </si>
+  <si>
+    <t xml:space="preserve">311
 312</t>
   </si>
   <si>
-    <t>Coolers: Quality</t>
-  </si>
-  <si>
-    <t>Холодильник: Качество</t>
-  </si>
-  <si>
-    <t>Local</t>
-  </si>
-  <si>
-    <t>LOCAL 6</t>
-  </si>
-  <si>
-    <t>Visible Cooler</t>
-  </si>
-  <si>
-    <t>Видимый ХО</t>
-  </si>
-  <si>
-    <t>number of atomic KPI Passed</t>
-  </si>
-  <si>
-    <t>Cooler</t>
+    <t xml:space="preserve">Coolers: Quality</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Холодильник: Качество</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Local</t>
+  </si>
+  <si>
+    <t xml:space="preserve">LOCAL 6</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Visible Cooler</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Видимый ХО</t>
+  </si>
+  <si>
+    <t xml:space="preserve">number of atomic KPI Passed</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Cooler</t>
   </si>
   <si>
     <t xml:space="preserve">34
@@ -420,55 +412,58 @@
 </t>
   </si>
   <si>
-    <t>Cooler is Visible</t>
-  </si>
-  <si>
-    <t>ХО виден</t>
-  </si>
-  <si>
-    <t>Scenes with no tagging</t>
-  </si>
-  <si>
-    <t>SCENES</t>
-  </si>
-  <si>
-    <t>Cooler fullness</t>
-  </si>
-  <si>
-    <t>ХО Заполнен</t>
-  </si>
-  <si>
-    <t>number of filled Coolers (scenes)</t>
-  </si>
-  <si>
-    <t>Manufacture: TCCC</t>
-  </si>
-  <si>
-    <t>TCCC</t>
-  </si>
-  <si>
-    <t>MAN</t>
-  </si>
-  <si>
-    <t>SOS with empty more than 80%</t>
-  </si>
-  <si>
-    <t>Cooler wo other products</t>
-  </si>
-  <si>
-    <t>ХО без посторонней продукции</t>
-  </si>
-  <si>
-    <t>number of pure Coolers</t>
-  </si>
-  <si>
-    <t>Share of TCCC product at least 98%</t>
-  </si>
-  <si>
-    <t>Activations</t>
-  </si>
-  <si>
-    <t>Активации</t>
+    <t xml:space="preserve">Cooler is Visible</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ХО виден</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Scenes with no tagging</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SCENES</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Panoramic photo of Cooler; SS_Panoramic photo of Cooler - Horeca</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Cooler fullness</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ХО Заполнен</t>
+  </si>
+  <si>
+    <t xml:space="preserve">number of filled Coolers (scenes)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Manufacture: TCCC</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TCCC</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MAN</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SOS with empty more than 80%</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Cooler wo other products</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ХО без посторонней продукции</t>
+  </si>
+  <si>
+    <t xml:space="preserve">number of pure Coolers</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Share of TCCC product at least 98%</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Activations</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Активации</t>
   </si>
   <si>
     <t xml:space="preserve">22
@@ -477,80 +472,89 @@
 </t>
   </si>
   <si>
-    <t>STANDARD 16</t>
-  </si>
-  <si>
-    <t>Menu Activation</t>
-  </si>
-  <si>
-    <t>Активация Меню</t>
-  </si>
-  <si>
-    <t>Brand: Schweppes, Rich, Burn,  Coca-Cola</t>
-  </si>
-  <si>
-    <t>Schweppes, Rich, Burn,  Coca-Cola</t>
-  </si>
-  <si>
-    <t>BRAND</t>
-  </si>
-  <si>
-    <t>STANDARD 17</t>
-  </si>
-  <si>
-    <t>Impulse Activation</t>
-  </si>
-  <si>
-    <t>Активация Импульсной зоны</t>
-  </si>
-  <si>
-    <t>Impulse Display</t>
-  </si>
-  <si>
-    <t>Импульс: Дисплей</t>
-  </si>
-  <si>
-    <t>Glass, glass, GLASS, Can, CAN, can</t>
-  </si>
-  <si>
-    <t>Destination Activation</t>
-  </si>
-  <si>
-    <t>Активация Стола</t>
+    <t xml:space="preserve">STANDARD 16</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Menu Activation</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Активация Меню</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Brand: Schweppes, Rich, Burn, Coca-Cola</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Schweppes, Rich, Burn, Coca-Cola</t>
+  </si>
+  <si>
+    <t xml:space="preserve">BRAND</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Other Menu Activation; Menu; Menu Insert; SS_Other Menu Activation; SS_Menu; SS_Menu Insert</t>
+  </si>
+  <si>
+    <t xml:space="preserve">STANDARD 17</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Impulse Activation</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Активация Импульсной зоны</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Bar Activation; SS_Bar Activation</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Impulse Display</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Импульс: Дисплей</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Glass, glass, GLASS, Can, CAN, can</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Destination Activation</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Активация Стола</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Table Activation; SS_Table Activation</t>
   </si>
   <si>
     <t xml:space="preserve">26
 </t>
   </si>
   <si>
-    <t>Destination: Images</t>
-  </si>
-  <si>
-    <t>Активация Стола: Имиджи</t>
-  </si>
-  <si>
-    <t>IC Activation</t>
-  </si>
-  <si>
-    <t>CAT</t>
-  </si>
-  <si>
-    <t>Hidden</t>
-  </si>
-  <si>
-    <t>VIS_COOLER_SAP</t>
-  </si>
-  <si>
-    <t>Visible cooler SAP</t>
-  </si>
-  <si>
-    <t>sum of atomic scores</t>
-  </si>
-  <si>
-    <t>Decimal.2</t>
-  </si>
-  <si>
-    <t>SESSION LEVEL</t>
+    <t xml:space="preserve">Destination: Images</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Активация Стола: Имиджи</t>
+  </si>
+  <si>
+    <t xml:space="preserve">IC Activation</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CAT</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Hidden</t>
+  </si>
+  <si>
+    <t xml:space="preserve">VIS_COOLER_SAP</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Visible cooler SAP</t>
+  </si>
+  <si>
+    <t xml:space="preserve">sum of atomic scores</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Decimal.2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SESSION LEVEL</t>
   </si>
   <si>
     <t xml:space="preserve">
@@ -560,103 +564,108 @@
 </t>
   </si>
   <si>
-    <t>CCH_PROD_MENU</t>
-  </si>
-  <si>
-    <t>CCH products present in Customer's menu</t>
-  </si>
-  <si>
-    <t>Passed or Failed Value</t>
-  </si>
-  <si>
-    <t>Text</t>
-  </si>
-  <si>
-    <t>MenuC1
+    <t xml:space="preserve">CCH_PROD_MENU</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CCH products present in Customer's menu</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Passed or Failed Value</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Text</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MenuC1
 No_MenuC1</t>
   </si>
   <si>
-    <t>ACTIVATION_SSD</t>
-  </si>
-  <si>
-    <t>Number of CCH activation points in SSD</t>
-  </si>
-  <si>
-    <t>IMPU
+    <t xml:space="preserve">ACTIVATION_SSD</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Number of CCH activation points in SSD</t>
+  </si>
+  <si>
+    <t xml:space="preserve">IMPU
 No_IMPU</t>
   </si>
   <si>
-    <t>DEST
+    <t xml:space="preserve">DEST
 No_DEST</t>
   </si>
   <si>
-    <t>OCCASIONS</t>
-  </si>
-  <si>
-    <t>PRIORITY_OCC</t>
-  </si>
-  <si>
-    <t>Number of Priority Occasions activated in the outlet</t>
-  </si>
-  <si>
-    <t>SEND VALUE if one KPI from lis is Passed , other No_O_A</t>
-  </si>
-  <si>
-    <t>EO
+    <t xml:space="preserve">OCCASIONS</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PRIORITY_OCC</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Number of Priority Occasions activated in the outlet</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SEND VALUE if one KPI from lis is Passed , other No_O_A</t>
+  </si>
+  <si>
+    <t xml:space="preserve">EO
 No_O_A</t>
   </si>
   <si>
-    <t>22
+    <t xml:space="preserve">22
 23
 25
 29</t>
   </si>
   <si>
-    <t>DO
+    <t xml:space="preserve">DO
 No_O_A</t>
   </si>
   <si>
-    <t>PLAN</t>
-  </si>
-  <si>
-    <t>Plan</t>
-  </si>
-  <si>
-    <t>Integer</t>
-  </si>
-  <si>
-    <t>Panoramic Photo; SS_Panoramic Photo</t>
-  </si>
-  <si>
-    <t>Panoramic photo of Cooler; SS_Panoramic photo of Cooler - Horeca</t>
-  </si>
-  <si>
-    <t>Other Menu Activation; Menu, Menu Insert; SS_Other Menu Activation; SS_Menu; SS_Menu Insert</t>
-  </si>
-  <si>
-    <t>Bar Activation; SS_Bar Activation</t>
-  </si>
-  <si>
-    <t>Table Activation; SS_Table Activation</t>
+    <t xml:space="preserve">PLAN</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Plan</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Integer</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="4">
-    <numFmt numFmtId="164" formatCode="_-* #,##0.00\ _₽_-;\-* #,##0.00\ _₽_-;_-* \-??\ _₽_-;_-@_-"/>
-    <numFmt numFmtId="165" formatCode="#,##0.0000000"/>
-    <numFmt numFmtId="166" formatCode="0.0%"/>
-    <numFmt numFmtId="167" formatCode="0.0"/>
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <numFmts count="9">
+    <numFmt numFmtId="164" formatCode="General"/>
+    <numFmt numFmtId="165" formatCode="0"/>
+    <numFmt numFmtId="166" formatCode="_-* #,##0.00\ _₽_-;\-* #,##0.00\ _₽_-;_-* \-??\ _₽_-;_-@_-"/>
+    <numFmt numFmtId="167" formatCode="#,##0.0000000"/>
+    <numFmt numFmtId="168" formatCode="0.00"/>
+    <numFmt numFmtId="169" formatCode="0%"/>
+    <numFmt numFmtId="170" formatCode="0.0%"/>
+    <numFmt numFmtId="171" formatCode="0.0"/>
+    <numFmt numFmtId="172" formatCode="@"/>
   </numFmts>
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="8">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
       <family val="2"/>
       <charset val="1"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <name val="Arial"/>
+      <family val="0"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <name val="Arial"/>
+      <family val="0"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <name val="Arial"/>
+      <family val="0"/>
     </font>
     <font>
       <sz val="11"/>
@@ -666,14 +675,14 @@
       <charset val="1"/>
     </font>
     <font>
-      <b/>
+      <b val="true"/>
       <sz val="11"/>
       <name val="Calibri"/>
       <family val="2"/>
       <charset val="1"/>
     </font>
     <font>
-      <b/>
+      <b val="true"/>
       <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
@@ -683,13 +692,6 @@
     <font>
       <sz val="11"/>
       <name val="Calibri"/>
-      <family val="2"/>
-      <charset val="1"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF000000"/>
-      <name val="Arial"/>
       <family val="2"/>
       <charset val="1"/>
     </font>
@@ -715,165 +717,189 @@
     </fill>
   </fills>
   <borders count="5">
-    <border>
+    <border diagonalUp="false" diagonalDown="false">
       <left/>
       <right/>
       <top/>
       <bottom/>
       <diagonal/>
     </border>
-    <border>
-      <left style="hair">
-        <color auto="1"/>
-      </left>
-      <right style="hair">
-        <color auto="1"/>
-      </right>
-      <top style="hair">
-        <color auto="1"/>
-      </top>
-      <bottom style="hair">
-        <color auto="1"/>
-      </bottom>
+    <border diagonalUp="false" diagonalDown="false">
+      <left style="hair"/>
+      <right style="hair"/>
+      <top style="hair"/>
+      <bottom style="hair"/>
       <diagonal/>
     </border>
-    <border>
-      <left style="hair">
-        <color auto="1"/>
-      </left>
+    <border diagonalUp="false" diagonalDown="false">
+      <left style="hair"/>
       <right/>
-      <top style="hair">
-        <color auto="1"/>
-      </top>
-      <bottom style="hair">
-        <color auto="1"/>
-      </bottom>
+      <top style="hair"/>
+      <bottom style="hair"/>
       <diagonal/>
     </border>
-    <border>
+    <border diagonalUp="false" diagonalDown="false">
       <left/>
-      <right style="hair">
-        <color auto="1"/>
-      </right>
-      <top style="hair">
-        <color auto="1"/>
-      </top>
-      <bottom style="hair">
-        <color auto="1"/>
-      </bottom>
+      <right style="hair"/>
+      <top style="hair"/>
+      <bottom style="hair"/>
       <diagonal/>
     </border>
-    <border>
-      <left style="dashed">
-        <color auto="1"/>
-      </left>
-      <right style="dashed">
-        <color auto="1"/>
-      </right>
-      <top style="dashed">
-        <color auto="1"/>
-      </top>
-      <bottom style="dashed">
-        <color auto="1"/>
-      </bottom>
+    <border diagonalUp="false" diagonalDown="false">
+      <left style="dashed"/>
+      <right style="dashed"/>
+      <top style="dashed"/>
+      <bottom style="dashed"/>
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="3">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" applyBorder="0" applyProtection="0"/>
-    <xf numFmtId="9" fontId="5" fillId="0" borderId="0" applyBorder="0" applyProtection="0"/>
+  <cellStyleXfs count="20">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
+    <xf numFmtId="41" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="169" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
   </cellStyleXfs>
-  <cellXfs count="28">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center"/>
+  <cellXfs count="27">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="1" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="3" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="165" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
+    <xf numFmtId="167" fontId="6" fillId="0" borderId="1" xfId="15" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="2" fontId="4" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
+    <xf numFmtId="164" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="1" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="168" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="1" fontId="4" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
+    <xf numFmtId="167" fontId="4" fillId="0" borderId="1" xfId="15" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="1" fontId="4" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    <xf numFmtId="165" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
+    <xf numFmtId="165" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    <xf numFmtId="164" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center"/>
-      <protection locked="0"/>
+    <xf numFmtId="164" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="166" fontId="4" fillId="0" borderId="1" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center"/>
+    <xf numFmtId="164" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="false" hidden="false"/>
     </xf>
-    <xf numFmtId="167" fontId="4" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
+    <xf numFmtId="170" fontId="7" fillId="0" borderId="1" xfId="19" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
+    <xf numFmtId="171" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="4" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="164" fontId="7" fillId="0" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center"/>
+    <xf numFmtId="167" fontId="7" fillId="0" borderId="1" xfId="15" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
+    <xf numFmtId="164" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="9" fontId="4" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
+    <xf numFmtId="169" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
+    <xf numFmtId="164" fontId="7" fillId="3" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
+    <xf numFmtId="164" fontId="4" fillId="3" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="49" fontId="4" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="172" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
-  <cellStyles count="3">
-    <cellStyle name="Comma" xfId="1" builtinId="3"/>
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Percent" xfId="2" builtinId="5"/>
+  <cellStyles count="6">
+    <cellStyle name="Normal" xfId="0" builtinId="0" customBuiltin="false"/>
+    <cellStyle name="Comma" xfId="15" builtinId="3" customBuiltin="false"/>
+    <cellStyle name="Comma [0]" xfId="16" builtinId="6" customBuiltin="false"/>
+    <cellStyle name="Currency" xfId="17" builtinId="4" customBuiltin="false"/>
+    <cellStyle name="Currency [0]" xfId="18" builtinId="7" customBuiltin="false"/>
+    <cellStyle name="Percent" xfId="19" builtinId="5" customBuiltin="false"/>
   </cellStyles>
-  <dxfs count="0"/>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
     <indexedColors>
       <rgbColor rgb="FF000000"/>
@@ -932,379 +958,75 @@
       <rgbColor rgb="FF993366"/>
       <rgbColor rgb="FF333399"/>
       <rgbColor rgb="FF333333"/>
-      <rgbColor rgb="00003366"/>
-      <rgbColor rgb="00339966"/>
-      <rgbColor rgb="00003300"/>
-      <rgbColor rgb="00333300"/>
-      <rgbColor rgb="00993300"/>
-      <rgbColor rgb="00993366"/>
-      <rgbColor rgb="00333399"/>
-      <rgbColor rgb="00333333"/>
     </indexedColors>
   </colors>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
-    </ext>
-  </extLst>
 </styleSheet>
 </file>
 
-<file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
-  <a:themeElements>
-    <a:clrScheme name="Office">
-      <a:dk1>
-        <a:sysClr val="windowText" lastClr="000000"/>
-      </a:dk1>
-      <a:lt1>
-        <a:sysClr val="window" lastClr="FFFFFF"/>
-      </a:lt1>
-      <a:dk2>
-        <a:srgbClr val="44546A"/>
-      </a:dk2>
-      <a:lt2>
-        <a:srgbClr val="E7E6E6"/>
-      </a:lt2>
-      <a:accent1>
-        <a:srgbClr val="4472C4"/>
-      </a:accent1>
-      <a:accent2>
-        <a:srgbClr val="ED7D31"/>
-      </a:accent2>
-      <a:accent3>
-        <a:srgbClr val="A5A5A5"/>
-      </a:accent3>
-      <a:accent4>
-        <a:srgbClr val="FFC000"/>
-      </a:accent4>
-      <a:accent5>
-        <a:srgbClr val="5B9BD5"/>
-      </a:accent5>
-      <a:accent6>
-        <a:srgbClr val="70AD47"/>
-      </a:accent6>
-      <a:hlink>
-        <a:srgbClr val="0563C1"/>
-      </a:hlink>
-      <a:folHlink>
-        <a:srgbClr val="954F72"/>
-      </a:folHlink>
-    </a:clrScheme>
-    <a:fontScheme name="Office">
-      <a:majorFont>
-        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
-        <a:ea typeface=""/>
-        <a:cs typeface=""/>
-        <a:font script="Jpan" typeface="游ゴシック Light"/>
-        <a:font script="Hang" typeface="맑은 고딕"/>
-        <a:font script="Hans" typeface="等线 Light"/>
-        <a:font script="Hant" typeface="新細明體"/>
-        <a:font script="Arab" typeface="Times New Roman"/>
-        <a:font script="Hebr" typeface="Times New Roman"/>
-        <a:font script="Thai" typeface="Tahoma"/>
-        <a:font script="Ethi" typeface="Nyala"/>
-        <a:font script="Beng" typeface="Vrinda"/>
-        <a:font script="Gujr" typeface="Shruti"/>
-        <a:font script="Khmr" typeface="MoolBoran"/>
-        <a:font script="Knda" typeface="Tunga"/>
-        <a:font script="Guru" typeface="Raavi"/>
-        <a:font script="Cans" typeface="Euphemia"/>
-        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
-        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
-        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
-        <a:font script="Thaa" typeface="MV Boli"/>
-        <a:font script="Deva" typeface="Mangal"/>
-        <a:font script="Telu" typeface="Gautami"/>
-        <a:font script="Taml" typeface="Latha"/>
-        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
-        <a:font script="Orya" typeface="Kalinga"/>
-        <a:font script="Mlym" typeface="Kartika"/>
-        <a:font script="Laoo" typeface="DokChampa"/>
-        <a:font script="Sinh" typeface="Iskoola Pota"/>
-        <a:font script="Mong" typeface="Mongolian Baiti"/>
-        <a:font script="Viet" typeface="Times New Roman"/>
-        <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
-      </a:majorFont>
-      <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
-        <a:ea typeface=""/>
-        <a:cs typeface=""/>
-        <a:font script="Jpan" typeface="游ゴシック"/>
-        <a:font script="Hang" typeface="맑은 고딕"/>
-        <a:font script="Hans" typeface="等线"/>
-        <a:font script="Hant" typeface="新細明體"/>
-        <a:font script="Arab" typeface="Arial"/>
-        <a:font script="Hebr" typeface="Arial"/>
-        <a:font script="Thai" typeface="Tahoma"/>
-        <a:font script="Ethi" typeface="Nyala"/>
-        <a:font script="Beng" typeface="Vrinda"/>
-        <a:font script="Gujr" typeface="Shruti"/>
-        <a:font script="Khmr" typeface="DaunPenh"/>
-        <a:font script="Knda" typeface="Tunga"/>
-        <a:font script="Guru" typeface="Raavi"/>
-        <a:font script="Cans" typeface="Euphemia"/>
-        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
-        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
-        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
-        <a:font script="Thaa" typeface="MV Boli"/>
-        <a:font script="Deva" typeface="Mangal"/>
-        <a:font script="Telu" typeface="Gautami"/>
-        <a:font script="Taml" typeface="Latha"/>
-        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
-        <a:font script="Orya" typeface="Kalinga"/>
-        <a:font script="Mlym" typeface="Kartika"/>
-        <a:font script="Laoo" typeface="DokChampa"/>
-        <a:font script="Sinh" typeface="Iskoola Pota"/>
-        <a:font script="Mong" typeface="Mongolian Baiti"/>
-        <a:font script="Viet" typeface="Arial"/>
-        <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
-      </a:minorFont>
-    </a:fontScheme>
-    <a:fmtScheme name="Office">
-      <a:fillStyleLst>
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
-        <a:gradFill rotWithShape="1">
-          <a:gsLst>
-            <a:gs pos="0">
-              <a:schemeClr val="phClr">
-                <a:lumMod val="110000"/>
-                <a:satMod val="105000"/>
-                <a:tint val="67000"/>
-              </a:schemeClr>
-            </a:gs>
-            <a:gs pos="50000">
-              <a:schemeClr val="phClr">
-                <a:lumMod val="105000"/>
-                <a:satMod val="103000"/>
-                <a:tint val="73000"/>
-              </a:schemeClr>
-            </a:gs>
-            <a:gs pos="100000">
-              <a:schemeClr val="phClr">
-                <a:lumMod val="105000"/>
-                <a:satMod val="109000"/>
-                <a:tint val="81000"/>
-              </a:schemeClr>
-            </a:gs>
-          </a:gsLst>
-          <a:lin ang="5400000" scaled="0"/>
-        </a:gradFill>
-        <a:gradFill rotWithShape="1">
-          <a:gsLst>
-            <a:gs pos="0">
-              <a:schemeClr val="phClr">
-                <a:satMod val="103000"/>
-                <a:lumMod val="102000"/>
-                <a:tint val="94000"/>
-              </a:schemeClr>
-            </a:gs>
-            <a:gs pos="50000">
-              <a:schemeClr val="phClr">
-                <a:satMod val="110000"/>
-                <a:lumMod val="100000"/>
-                <a:shade val="100000"/>
-              </a:schemeClr>
-            </a:gs>
-            <a:gs pos="100000">
-              <a:schemeClr val="phClr">
-                <a:lumMod val="99000"/>
-                <a:satMod val="120000"/>
-                <a:shade val="78000"/>
-              </a:schemeClr>
-            </a:gs>
-          </a:gsLst>
-          <a:lin ang="5400000" scaled="0"/>
-        </a:gradFill>
-      </a:fillStyleLst>
-      <a:lnStyleLst>
-        <a:ln w="6350" cap="flat" cmpd="sng" algn="ctr">
-          <a:solidFill>
-            <a:schemeClr val="phClr"/>
-          </a:solidFill>
-          <a:prstDash val="solid"/>
-          <a:miter lim="800000"/>
-        </a:ln>
-        <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
-          <a:solidFill>
-            <a:schemeClr val="phClr"/>
-          </a:solidFill>
-          <a:prstDash val="solid"/>
-          <a:miter lim="800000"/>
-        </a:ln>
-        <a:ln w="19050" cap="flat" cmpd="sng" algn="ctr">
-          <a:solidFill>
-            <a:schemeClr val="phClr"/>
-          </a:solidFill>
-          <a:prstDash val="solid"/>
-          <a:miter lim="800000"/>
-        </a:ln>
-      </a:lnStyleLst>
-      <a:effectStyleLst>
-        <a:effectStyle>
-          <a:effectLst/>
-        </a:effectStyle>
-        <a:effectStyle>
-          <a:effectLst/>
-        </a:effectStyle>
-        <a:effectStyle>
-          <a:effectLst>
-            <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
-              <a:srgbClr val="000000">
-                <a:alpha val="63000"/>
-              </a:srgbClr>
-            </a:outerShdw>
-          </a:effectLst>
-        </a:effectStyle>
-      </a:effectStyleLst>
-      <a:bgFillStyleLst>
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
-        <a:solidFill>
-          <a:schemeClr val="phClr">
-            <a:tint val="95000"/>
-            <a:satMod val="170000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:gradFill rotWithShape="1">
-          <a:gsLst>
-            <a:gs pos="0">
-              <a:schemeClr val="phClr">
-                <a:tint val="93000"/>
-                <a:satMod val="150000"/>
-                <a:shade val="98000"/>
-                <a:lumMod val="102000"/>
-              </a:schemeClr>
-            </a:gs>
-            <a:gs pos="50000">
-              <a:schemeClr val="phClr">
-                <a:tint val="98000"/>
-                <a:satMod val="130000"/>
-                <a:shade val="90000"/>
-                <a:lumMod val="103000"/>
-              </a:schemeClr>
-            </a:gs>
-            <a:gs pos="100000">
-              <a:schemeClr val="phClr">
-                <a:shade val="63000"/>
-                <a:satMod val="120000"/>
-              </a:schemeClr>
-            </a:gs>
-          </a:gsLst>
-          <a:lin ang="5400000" scaled="0"/>
-        </a:gradFill>
-      </a:bgFillStyleLst>
-    </a:fmtScheme>
-  </a:themeElements>
-  <a:objectDefaults/>
-  <a:extraClrSchemeLst/>
-  <a:extLst>
-    <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
-    </a:ext>
-  </a:extLst>
-</a:theme>
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships"/>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:AMK39"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:AO39"/>
   <sheetViews>
-    <sheetView windowProtection="1" tabSelected="1" zoomScale="65" zoomScaleNormal="65" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection activeCell="T1" sqref="T1"/>
-      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
+    <sheetView windowProtection="true" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="U1" colorId="64" zoomScale="65" zoomScaleNormal="65" zoomScalePageLayoutView="100" workbookViewId="0">
+      <pane xSplit="0" ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="topLeft" activeCell="U1" activeCellId="0" sqref="U1"/>
+      <selection pane="bottomLeft" activeCell="AC29" activeCellId="0" sqref="AC29"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="13.5" style="1"/>
-    <col min="2" max="2" width="16.5" style="1"/>
-    <col min="3" max="3" width="37.796875" style="1"/>
-    <col min="4" max="4" width="15.19921875" style="1"/>
-    <col min="5" max="5" width="17.09765625" style="1"/>
-    <col min="6" max="6" width="64.3984375" style="1"/>
-    <col min="7" max="7" width="68.8984375" style="1"/>
-    <col min="8" max="8" width="38.8984375" style="1"/>
-    <col min="9" max="9" width="24" style="1"/>
-    <col min="10" max="10" width="24.5" style="1"/>
-    <col min="11" max="11" width="22" style="1"/>
-    <col min="12" max="12" width="12.296875" style="1"/>
-    <col min="13" max="13" width="18.09765625" style="1"/>
-    <col min="14" max="14" width="18.796875" style="1"/>
-    <col min="15" max="15" width="64.3984375" style="1"/>
-    <col min="16" max="16" width="53.296875" style="1"/>
-    <col min="17" max="17" width="26.09765625" style="1"/>
-    <col min="18" max="18" width="21.5" style="1"/>
-    <col min="19" max="19" width="21.09765625" style="1"/>
-    <col min="20" max="20" width="40" style="1"/>
-    <col min="21" max="21" width="25.19921875" style="1"/>
-    <col min="22" max="22" width="18.59765625" style="1"/>
-    <col min="23" max="23" width="9.69921875" style="1"/>
-    <col min="24" max="24" width="41" style="1"/>
-    <col min="25" max="25" width="29.3984375" style="1"/>
-    <col min="26" max="26" width="23.59765625" style="1"/>
-    <col min="27" max="27" width="30.296875" style="1"/>
-    <col min="28" max="28" width="29.5" style="1"/>
-    <col min="29" max="29" width="83.5" style="1" bestFit="1" customWidth="1"/>
-    <col min="30" max="30" width="27.19921875" style="1"/>
-    <col min="31" max="31" width="34.09765625" style="1"/>
-    <col min="32" max="32" width="34.59765625" style="1"/>
-    <col min="33" max="33" width="22.3984375" style="1"/>
-    <col min="34" max="34" width="18.3984375" style="1"/>
-    <col min="35" max="35" width="16.8984375" style="1"/>
-    <col min="36" max="36" width="17.59765625" style="1"/>
-    <col min="37" max="37" width="41.09765625" style="1"/>
-    <col min="38" max="38" width="10.3984375" style="1"/>
-    <col min="39" max="39" width="12.19921875" style="1"/>
-    <col min="40" max="40" width="14.796875" style="1"/>
-    <col min="41" max="41" width="12.69921875" style="1"/>
-    <col min="42" max="1025" width="12.19921875" style="1"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="14.8325581395349"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="18.1162790697674"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="41.4790697674419"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="16.6697674418605"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="1" width="18.7720930232558"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="1" width="70.753488372093"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="1" width="75.6093023255814"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="1" width="42.6604651162791"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="1" width="26.3860465116279"/>
+    <col collapsed="false" hidden="false" max="10" min="10" style="1" width="26.9116279069767"/>
+    <col collapsed="false" hidden="false" max="11" min="11" style="1" width="24.153488372093"/>
+    <col collapsed="false" hidden="false" max="12" min="12" style="1" width="13.3906976744186"/>
+    <col collapsed="false" hidden="false" max="13" min="13" style="1" width="19.8232558139535"/>
+    <col collapsed="false" hidden="false" max="14" min="14" style="1" width="20.6093023255814"/>
+    <col collapsed="false" hidden="false" max="15" min="15" style="1" width="70.753488372093"/>
+    <col collapsed="false" hidden="false" max="16" min="16" style="1" width="58.5441860465116"/>
+    <col collapsed="false" hidden="false" max="17" min="17" style="1" width="28.6139534883721"/>
+    <col collapsed="false" hidden="false" max="18" min="18" style="1" width="23.6279069767442"/>
+    <col collapsed="false" hidden="false" max="19" min="19" style="1" width="23.1023255813953"/>
+    <col collapsed="false" hidden="false" max="20" min="20" style="1" width="43.9720930232558"/>
+    <col collapsed="false" hidden="false" max="21" min="21" style="1" width="27.6976744186047"/>
+    <col collapsed="false" hidden="false" max="22" min="22" style="1" width="20.4790697674419"/>
+    <col collapsed="false" hidden="false" max="23" min="23" style="1" width="10.6325581395349"/>
+    <col collapsed="false" hidden="false" max="24" min="24" style="1" width="45.0232558139535"/>
+    <col collapsed="false" hidden="false" max="25" min="25" style="1" width="32.293023255814"/>
+    <col collapsed="false" hidden="false" max="26" min="26" style="1" width="25.8604651162791"/>
+    <col collapsed="false" hidden="false" max="27" min="27" style="1" width="33.2093023255814"/>
+    <col collapsed="false" hidden="false" max="28" min="28" style="1" width="32.4232558139535"/>
+    <col collapsed="false" hidden="false" max="29" min="29" style="1" width="91.753488372093"/>
+    <col collapsed="false" hidden="false" max="30" min="30" style="1" width="29.9302325581395"/>
+    <col collapsed="false" hidden="false" max="31" min="31" style="1" width="37.4093023255814"/>
+    <col collapsed="false" hidden="false" max="32" min="32" style="1" width="38.0651162790698"/>
+    <col collapsed="false" hidden="false" max="33" min="33" style="1" width="24.5488372093023"/>
+    <col collapsed="false" hidden="false" max="34" min="34" style="1" width="20.0837209302326"/>
+    <col collapsed="false" hidden="false" max="35" min="35" style="1" width="18.506976744186"/>
+    <col collapsed="false" hidden="false" max="36" min="36" style="1" width="19.2976744186047"/>
+    <col collapsed="false" hidden="false" max="37" min="37" style="1" width="45.153488372093"/>
+    <col collapsed="false" hidden="false" max="38" min="38" style="1" width="11.2883720930233"/>
+    <col collapsed="false" hidden="false" max="39" min="39" style="1" width="13.3906976744186"/>
+    <col collapsed="false" hidden="false" max="40" min="40" style="1" width="16.1441860465116"/>
+    <col collapsed="false" hidden="false" max="41" min="41" style="1" width="13.9162790697674"/>
+    <col collapsed="false" hidden="false" max="1025" min="42" style="1" width="13.3906976744186"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:41" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" customFormat="false" ht="21.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -1429,8 +1151,8 @@
         <v>40</v>
       </c>
     </row>
-    <row r="2" spans="1:41" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="7">
+    <row r="2" customFormat="false" ht="21.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A2" s="7" t="n">
         <v>41</v>
       </c>
       <c r="B2" s="7" t="s">
@@ -1481,10 +1203,10 @@
       <c r="AI2" s="7"/>
       <c r="AJ2" s="7"/>
       <c r="AK2" s="7"/>
-      <c r="AL2" s="10">
+      <c r="AL2" s="10" t="n">
         <v>1</v>
       </c>
-      <c r="AM2" s="10">
+      <c r="AM2" s="10" t="n">
         <v>300</v>
       </c>
       <c r="AN2" s="11" t="s">
@@ -1492,8 +1214,8 @@
       </c>
       <c r="AO2" s="7"/>
     </row>
-    <row r="3" spans="1:41" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="7">
+    <row r="3" customFormat="false" ht="21.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A3" s="7" t="n">
         <v>1</v>
       </c>
       <c r="B3" s="7" t="s">
@@ -1552,21 +1274,21 @@
       <c r="AI3" s="7"/>
       <c r="AJ3" s="7"/>
       <c r="AK3" s="7"/>
-      <c r="AL3" s="7">
+      <c r="AL3" s="7" t="n">
         <v>2</v>
       </c>
-      <c r="AM3" s="7">
+      <c r="AM3" s="7" t="n">
         <v>1</v>
       </c>
       <c r="AN3" s="13" t="s">
         <v>53</v>
       </c>
-      <c r="AO3" s="7">
+      <c r="AO3" s="7" t="n">
         <v>300</v>
       </c>
     </row>
-    <row r="4" spans="1:41" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="7">
+    <row r="4" customFormat="false" ht="21.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A4" s="7" t="n">
         <v>2</v>
       </c>
       <c r="B4" s="7" t="s">
@@ -1593,7 +1315,7 @@
       <c r="I4" s="7"/>
       <c r="J4" s="7"/>
       <c r="K4" s="7"/>
-      <c r="L4" s="7">
+      <c r="L4" s="7" t="n">
         <v>1</v>
       </c>
       <c r="M4" s="7"/>
@@ -1601,7 +1323,7 @@
       <c r="O4" s="7" t="s">
         <v>54</v>
       </c>
-      <c r="P4" s="10">
+      <c r="P4" s="10" t="n">
         <v>50112128</v>
       </c>
       <c r="Q4" s="10"/>
@@ -1624,32 +1346,32 @@
       <c r="AB4" s="7"/>
       <c r="AC4" s="7"/>
       <c r="AD4" s="7" t="s">
-        <v>184</v>
+        <v>60</v>
       </c>
       <c r="AE4" s="7"/>
       <c r="AF4" s="7"/>
       <c r="AG4" s="7" t="s">
-        <v>60</v>
-      </c>
-      <c r="AH4" s="9">
-        <v>6.5007999999999996E-2</v>
+        <v>61</v>
+      </c>
+      <c r="AH4" s="9" t="n">
+        <v>0.065008</v>
       </c>
       <c r="AI4" s="7"/>
       <c r="AJ4" s="7"/>
       <c r="AK4" s="7"/>
-      <c r="AL4" s="7">
+      <c r="AL4" s="7" t="n">
         <v>3</v>
       </c>
-      <c r="AM4" s="7">
+      <c r="AM4" s="7" t="n">
         <v>2</v>
       </c>
       <c r="AN4" s="7"/>
-      <c r="AO4" s="7">
+      <c r="AO4" s="7" t="n">
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:41" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="7">
+    <row r="5" customFormat="false" ht="21.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A5" s="7" t="n">
         <v>4</v>
       </c>
       <c r="B5" s="7" t="s">
@@ -1665,10 +1387,10 @@
         <v>47</v>
       </c>
       <c r="F5" s="7" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="G5" s="14" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="H5" s="7" t="s">
         <v>56</v>
@@ -1676,15 +1398,15 @@
       <c r="I5" s="7"/>
       <c r="J5" s="7"/>
       <c r="K5" s="7"/>
-      <c r="L5" s="7">
+      <c r="L5" s="7" t="n">
         <v>1</v>
       </c>
       <c r="M5" s="7"/>
       <c r="N5" s="7"/>
       <c r="O5" s="7" t="s">
-        <v>61</v>
-      </c>
-      <c r="P5" s="10">
+        <v>62</v>
+      </c>
+      <c r="P5" s="10" t="n">
         <v>90375408</v>
       </c>
       <c r="Q5" s="10"/>
@@ -1707,32 +1429,32 @@
       <c r="AB5" s="7"/>
       <c r="AC5" s="7"/>
       <c r="AD5" s="7" t="s">
-        <v>184</v>
+        <v>60</v>
       </c>
       <c r="AE5" s="7"/>
       <c r="AF5" s="7"/>
       <c r="AG5" s="7" t="s">
-        <v>60</v>
-      </c>
-      <c r="AH5" s="9">
-        <v>6.5007999999999996E-2</v>
+        <v>61</v>
+      </c>
+      <c r="AH5" s="9" t="n">
+        <v>0.065008</v>
       </c>
       <c r="AI5" s="7"/>
       <c r="AJ5" s="7"/>
       <c r="AK5" s="7"/>
-      <c r="AL5" s="7">
+      <c r="AL5" s="7" t="n">
         <v>3</v>
       </c>
-      <c r="AM5" s="7">
+      <c r="AM5" s="7" t="n">
         <v>4</v>
       </c>
       <c r="AN5" s="7"/>
-      <c r="AO5" s="7">
+      <c r="AO5" s="7" t="n">
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:41" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="7">
+    <row r="6" customFormat="false" ht="21.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A6" s="7" t="n">
         <v>3</v>
       </c>
       <c r="B6" s="7" t="s">
@@ -1748,10 +1470,10 @@
         <v>47</v>
       </c>
       <c r="F6" s="14" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="G6" s="14" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="H6" s="7" t="s">
         <v>56</v>
@@ -1759,15 +1481,15 @@
       <c r="I6" s="7"/>
       <c r="J6" s="7"/>
       <c r="K6" s="7"/>
-      <c r="L6" s="7">
+      <c r="L6" s="7" t="n">
         <v>1</v>
       </c>
       <c r="M6" s="7"/>
       <c r="N6" s="7"/>
       <c r="O6" s="14" t="s">
-        <v>63</v>
-      </c>
-      <c r="P6" s="10">
+        <v>64</v>
+      </c>
+      <c r="P6" s="10" t="n">
         <v>40822341</v>
       </c>
       <c r="Q6" s="10"/>
@@ -1790,32 +1512,32 @@
       <c r="AB6" s="7"/>
       <c r="AC6" s="7"/>
       <c r="AD6" s="7" t="s">
-        <v>184</v>
+        <v>60</v>
       </c>
       <c r="AE6" s="7"/>
       <c r="AF6" s="7"/>
       <c r="AG6" s="7" t="s">
-        <v>60</v>
-      </c>
-      <c r="AH6" s="9">
-        <v>6.5007999999999996E-2</v>
+        <v>61</v>
+      </c>
+      <c r="AH6" s="9" t="n">
+        <v>0.065008</v>
       </c>
       <c r="AI6" s="7"/>
       <c r="AJ6" s="7"/>
       <c r="AK6" s="7"/>
-      <c r="AL6" s="7">
+      <c r="AL6" s="7" t="n">
         <v>3</v>
       </c>
-      <c r="AM6" s="7">
+      <c r="AM6" s="7" t="n">
         <v>3</v>
       </c>
       <c r="AN6" s="7"/>
-      <c r="AO6" s="7">
+      <c r="AO6" s="7" t="n">
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:41" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="7">
+    <row r="7" customFormat="false" ht="21.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A7" s="7" t="n">
         <v>5</v>
       </c>
       <c r="B7" s="7" t="s">
@@ -1831,10 +1553,10 @@
         <v>47</v>
       </c>
       <c r="F7" s="14" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="G7" s="14" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="H7" s="7" t="s">
         <v>56</v>
@@ -1842,15 +1564,15 @@
       <c r="I7" s="7"/>
       <c r="J7" s="7"/>
       <c r="K7" s="7"/>
-      <c r="L7" s="7">
+      <c r="L7" s="7" t="n">
         <v>1</v>
       </c>
       <c r="M7" s="7"/>
       <c r="N7" s="7"/>
       <c r="O7" s="14" t="s">
-        <v>65</v>
-      </c>
-      <c r="P7" s="10">
+        <v>66</v>
+      </c>
+      <c r="P7" s="10" t="n">
         <v>40822549</v>
       </c>
       <c r="Q7" s="10"/>
@@ -1873,32 +1595,32 @@
       <c r="AB7" s="7"/>
       <c r="AC7" s="7"/>
       <c r="AD7" s="7" t="s">
-        <v>184</v>
+        <v>60</v>
       </c>
       <c r="AE7" s="7"/>
       <c r="AF7" s="7"/>
       <c r="AG7" s="7" t="s">
-        <v>60</v>
-      </c>
-      <c r="AH7" s="9">
-        <v>6.5007999999999996E-2</v>
+        <v>61</v>
+      </c>
+      <c r="AH7" s="9" t="n">
+        <v>0.065008</v>
       </c>
       <c r="AI7" s="7"/>
       <c r="AJ7" s="7"/>
       <c r="AK7" s="7"/>
-      <c r="AL7" s="7">
+      <c r="AL7" s="7" t="n">
         <v>3</v>
       </c>
-      <c r="AM7" s="7">
+      <c r="AM7" s="7" t="n">
         <v>5</v>
       </c>
       <c r="AN7" s="7"/>
-      <c r="AO7" s="7">
+      <c r="AO7" s="7" t="n">
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:41" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="7">
+    <row r="8" customFormat="false" ht="21.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A8" s="7" t="n">
         <v>8</v>
       </c>
       <c r="B8" s="7" t="s">
@@ -1914,10 +1636,10 @@
         <v>47</v>
       </c>
       <c r="F8" s="14" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="G8" s="14" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="H8" s="7" t="s">
         <v>56</v>
@@ -1925,16 +1647,16 @@
       <c r="I8" s="7"/>
       <c r="J8" s="7"/>
       <c r="K8" s="7"/>
-      <c r="L8" s="7">
+      <c r="L8" s="7" t="n">
         <v>1</v>
       </c>
       <c r="M8" s="7"/>
       <c r="N8" s="7"/>
       <c r="O8" s="14" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="P8" s="14" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="Q8" s="10"/>
       <c r="R8" s="10"/>
@@ -1956,32 +1678,32 @@
       <c r="AB8" s="7"/>
       <c r="AC8" s="7"/>
       <c r="AD8" s="7" t="s">
-        <v>184</v>
+        <v>60</v>
       </c>
       <c r="AE8" s="7"/>
       <c r="AF8" s="7"/>
       <c r="AG8" s="7" t="s">
-        <v>60</v>
-      </c>
-      <c r="AH8" s="9">
-        <v>2.5965999999999999E-2</v>
+        <v>61</v>
+      </c>
+      <c r="AH8" s="9" t="n">
+        <v>0.025966</v>
       </c>
       <c r="AI8" s="7"/>
       <c r="AJ8" s="7"/>
       <c r="AK8" s="7"/>
-      <c r="AL8" s="7">
+      <c r="AL8" s="7" t="n">
         <v>3</v>
       </c>
-      <c r="AM8" s="7">
+      <c r="AM8" s="7" t="n">
         <v>8</v>
       </c>
       <c r="AN8" s="7"/>
-      <c r="AO8" s="7">
+      <c r="AO8" s="7" t="n">
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:41" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="7">
+    <row r="9" customFormat="false" ht="21.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A9" s="7" t="n">
         <v>9</v>
       </c>
       <c r="B9" s="7" t="s">
@@ -1994,13 +1716,13 @@
         <v>43</v>
       </c>
       <c r="E9" s="7" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="F9" s="7" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="G9" s="7" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="H9" s="7" t="s">
         <v>50</v>
@@ -2009,7 +1731,7 @@
         <v>44</v>
       </c>
       <c r="J9" s="12" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="K9" s="7"/>
       <c r="L9" s="7"/>
@@ -2042,21 +1764,21 @@
       <c r="AI9" s="7"/>
       <c r="AJ9" s="7"/>
       <c r="AK9" s="7"/>
-      <c r="AL9" s="7">
+      <c r="AL9" s="7" t="n">
         <v>2</v>
       </c>
-      <c r="AM9" s="7">
+      <c r="AM9" s="7" t="n">
         <v>9</v>
       </c>
-      <c r="AN9" s="7">
+      <c r="AN9" s="7" t="n">
         <v>10</v>
       </c>
-      <c r="AO9" s="7">
+      <c r="AO9" s="7" t="n">
         <v>300</v>
       </c>
     </row>
-    <row r="10" spans="1:41" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="7">
+    <row r="10" customFormat="false" ht="21.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A10" s="7" t="n">
         <v>10</v>
       </c>
       <c r="B10" s="7" t="s">
@@ -2069,13 +1791,13 @@
         <v>43</v>
       </c>
       <c r="E10" s="7" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="F10" s="14" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="G10" s="14" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="H10" s="7" t="s">
         <v>56</v>
@@ -2083,16 +1805,16 @@
       <c r="I10" s="7"/>
       <c r="J10" s="7"/>
       <c r="K10" s="7"/>
-      <c r="L10" s="7">
+      <c r="L10" s="7" t="n">
         <v>1</v>
       </c>
       <c r="M10" s="7"/>
       <c r="N10" s="7"/>
       <c r="O10" s="14" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="P10" s="10" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="Q10" s="10"/>
       <c r="R10" s="10"/>
@@ -2114,32 +1836,32 @@
       <c r="AB10" s="7"/>
       <c r="AC10" s="7"/>
       <c r="AD10" s="7" t="s">
-        <v>184</v>
+        <v>60</v>
       </c>
       <c r="AE10" s="7"/>
       <c r="AF10" s="7"/>
       <c r="AG10" s="7" t="s">
-        <v>60</v>
-      </c>
-      <c r="AH10" s="9">
-        <v>6.2417E-2</v>
+        <v>61</v>
+      </c>
+      <c r="AH10" s="9" t="n">
+        <v>0.062417</v>
       </c>
       <c r="AI10" s="15"/>
       <c r="AJ10" s="7"/>
       <c r="AK10" s="7"/>
-      <c r="AL10" s="7">
+      <c r="AL10" s="7" t="n">
         <v>3</v>
       </c>
-      <c r="AM10" s="7">
+      <c r="AM10" s="7" t="n">
         <v>10</v>
       </c>
       <c r="AN10" s="7"/>
-      <c r="AO10" s="7">
+      <c r="AO10" s="7" t="n">
         <v>9</v>
       </c>
     </row>
-    <row r="11" spans="1:41" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="7">
+    <row r="11" customFormat="false" ht="21.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A11" s="7" t="n">
         <v>11</v>
       </c>
       <c r="B11" s="7" t="s">
@@ -2152,13 +1874,13 @@
         <v>43</v>
       </c>
       <c r="E11" s="7" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="F11" s="7" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="G11" s="7" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="H11" s="7" t="s">
         <v>50</v>
@@ -2167,7 +1889,7 @@
         <v>44</v>
       </c>
       <c r="J11" s="12" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="K11" s="7"/>
       <c r="L11" s="7"/>
@@ -2200,21 +1922,21 @@
       <c r="AI11" s="7"/>
       <c r="AJ11" s="7"/>
       <c r="AK11" s="7"/>
-      <c r="AL11" s="7">
+      <c r="AL11" s="7" t="n">
         <v>2</v>
       </c>
-      <c r="AM11" s="7">
+      <c r="AM11" s="7" t="n">
         <v>11</v>
       </c>
       <c r="AN11" s="13" t="s">
-        <v>82</v>
-      </c>
-      <c r="AO11" s="7">
+        <v>83</v>
+      </c>
+      <c r="AO11" s="7" t="n">
         <v>300</v>
       </c>
     </row>
-    <row r="12" spans="1:41" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="7">
+    <row r="12" customFormat="false" ht="21.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A12" s="7" t="n">
         <v>12</v>
       </c>
       <c r="B12" s="7" t="s">
@@ -2227,13 +1949,13 @@
         <v>43</v>
       </c>
       <c r="E12" s="7" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="F12" s="7" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="G12" s="14" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="H12" s="7" t="s">
         <v>56</v>
@@ -2241,15 +1963,15 @@
       <c r="I12" s="7"/>
       <c r="J12" s="7"/>
       <c r="K12" s="7"/>
-      <c r="L12" s="7">
+      <c r="L12" s="7" t="n">
         <v>1</v>
       </c>
       <c r="M12" s="7"/>
       <c r="N12" s="7"/>
       <c r="O12" s="7" t="s">
-        <v>83</v>
-      </c>
-      <c r="P12" s="10">
+        <v>84</v>
+      </c>
+      <c r="P12" s="10" t="n">
         <v>4650075420386</v>
       </c>
       <c r="Q12" s="10"/>
@@ -2272,32 +1994,32 @@
       <c r="AB12" s="7"/>
       <c r="AC12" s="7"/>
       <c r="AD12" s="7" t="s">
-        <v>184</v>
+        <v>60</v>
       </c>
       <c r="AE12" s="7"/>
       <c r="AF12" s="7"/>
       <c r="AG12" s="7" t="s">
-        <v>60</v>
-      </c>
-      <c r="AH12" s="9">
-        <v>3.0317E-2</v>
+        <v>61</v>
+      </c>
+      <c r="AH12" s="9" t="n">
+        <v>0.030317</v>
       </c>
       <c r="AI12" s="7"/>
       <c r="AJ12" s="7"/>
       <c r="AK12" s="7"/>
-      <c r="AL12" s="7">
+      <c r="AL12" s="7" t="n">
         <v>3</v>
       </c>
-      <c r="AM12" s="7">
+      <c r="AM12" s="7" t="n">
         <v>12</v>
       </c>
       <c r="AN12" s="7"/>
-      <c r="AO12" s="7">
+      <c r="AO12" s="7" t="n">
         <v>11</v>
       </c>
     </row>
-    <row r="13" spans="1:41" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="7">
+    <row r="13" customFormat="false" ht="21.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A13" s="7" t="n">
         <v>13</v>
       </c>
       <c r="B13" s="7" t="s">
@@ -2310,13 +2032,13 @@
         <v>43</v>
       </c>
       <c r="E13" s="7" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="F13" s="7" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="G13" s="14" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="H13" s="7" t="s">
         <v>56</v>
@@ -2324,15 +2046,15 @@
       <c r="I13" s="7"/>
       <c r="J13" s="7"/>
       <c r="K13" s="7"/>
-      <c r="L13" s="7">
+      <c r="L13" s="7" t="n">
         <v>1</v>
       </c>
       <c r="M13" s="7"/>
       <c r="N13" s="7"/>
       <c r="O13" s="7" t="s">
-        <v>85</v>
-      </c>
-      <c r="P13" s="10">
+        <v>86</v>
+      </c>
+      <c r="P13" s="10" t="n">
         <v>4650075420362</v>
       </c>
       <c r="Q13" s="10"/>
@@ -2355,32 +2077,32 @@
       <c r="AB13" s="7"/>
       <c r="AC13" s="7"/>
       <c r="AD13" s="7" t="s">
-        <v>184</v>
+        <v>60</v>
       </c>
       <c r="AE13" s="7"/>
       <c r="AF13" s="7"/>
       <c r="AG13" s="7" t="s">
-        <v>60</v>
-      </c>
-      <c r="AH13" s="9">
-        <v>3.0317E-2</v>
+        <v>61</v>
+      </c>
+      <c r="AH13" s="9" t="n">
+        <v>0.030317</v>
       </c>
       <c r="AI13" s="7"/>
       <c r="AJ13" s="7"/>
       <c r="AK13" s="7"/>
-      <c r="AL13" s="7">
+      <c r="AL13" s="7" t="n">
         <v>3</v>
       </c>
-      <c r="AM13" s="7">
+      <c r="AM13" s="7" t="n">
         <v>13</v>
       </c>
       <c r="AN13" s="7"/>
-      <c r="AO13" s="7">
+      <c r="AO13" s="7" t="n">
         <v>11</v>
       </c>
     </row>
-    <row r="14" spans="1:41" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="7">
+    <row r="14" customFormat="false" ht="21.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A14" s="7" t="n">
         <v>14</v>
       </c>
       <c r="B14" s="7" t="s">
@@ -2393,21 +2115,21 @@
         <v>43</v>
       </c>
       <c r="E14" s="7" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="F14" s="7" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="G14" s="14" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="H14" s="7" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="I14" s="7"/>
       <c r="J14" s="7"/>
       <c r="K14" s="7"/>
-      <c r="L14" s="7">
+      <c r="L14" s="7" t="n">
         <v>1</v>
       </c>
       <c r="M14" s="7"/>
@@ -2430,34 +2152,34 @@
       <c r="AB14" s="7"/>
       <c r="AC14" s="7"/>
       <c r="AD14" s="7" t="s">
-        <v>184</v>
+        <v>60</v>
       </c>
       <c r="AE14" s="7"/>
       <c r="AF14" s="7"/>
       <c r="AG14" s="7" t="s">
-        <v>60</v>
-      </c>
-      <c r="AH14" s="9">
-        <v>3.0317E-2</v>
+        <v>61</v>
+      </c>
+      <c r="AH14" s="9" t="n">
+        <v>0.030317</v>
       </c>
       <c r="AI14" s="7"/>
       <c r="AJ14" s="7"/>
       <c r="AK14" s="7"/>
-      <c r="AL14" s="7">
+      <c r="AL14" s="7" t="n">
         <v>3</v>
       </c>
-      <c r="AM14" s="7">
+      <c r="AM14" s="7" t="n">
         <v>15</v>
       </c>
       <c r="AN14" s="13" t="s">
-        <v>90</v>
-      </c>
-      <c r="AO14" s="7">
+        <v>91</v>
+      </c>
+      <c r="AO14" s="7" t="n">
         <v>11</v>
       </c>
     </row>
-    <row r="15" spans="1:41" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="7">
+    <row r="15" customFormat="false" ht="21.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A15" s="7" t="n">
         <v>16</v>
       </c>
       <c r="B15" s="7" t="s">
@@ -2470,13 +2192,13 @@
         <v>43</v>
       </c>
       <c r="E15" s="7" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="F15" s="7" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="G15" s="14" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="H15" s="7" t="s">
         <v>56</v>
@@ -2484,15 +2206,15 @@
       <c r="I15" s="7"/>
       <c r="J15" s="7"/>
       <c r="K15" s="7"/>
-      <c r="L15" s="7">
+      <c r="L15" s="7" t="n">
         <v>1</v>
       </c>
       <c r="M15" s="7"/>
       <c r="N15" s="7"/>
       <c r="O15" s="7" t="s">
-        <v>91</v>
-      </c>
-      <c r="P15" s="10">
+        <v>92</v>
+      </c>
+      <c r="P15" s="10" t="n">
         <v>4650075420423</v>
       </c>
       <c r="Q15" s="10"/>
@@ -2515,30 +2237,30 @@
       <c r="AB15" s="7"/>
       <c r="AC15" s="7"/>
       <c r="AD15" s="7" t="s">
-        <v>184</v>
+        <v>60</v>
       </c>
       <c r="AE15" s="7"/>
       <c r="AF15" s="7"/>
       <c r="AG15" s="7" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="AH15" s="9"/>
       <c r="AI15" s="7"/>
       <c r="AJ15" s="7"/>
       <c r="AK15" s="7"/>
-      <c r="AL15" s="7">
+      <c r="AL15" s="7" t="n">
         <v>4</v>
       </c>
-      <c r="AM15" s="7">
+      <c r="AM15" s="7" t="n">
         <v>17</v>
       </c>
       <c r="AN15" s="7"/>
-      <c r="AO15" s="13">
+      <c r="AO15" s="13" t="n">
         <v>15</v>
       </c>
     </row>
-    <row r="16" spans="1:41" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="7">
+    <row r="16" customFormat="false" ht="21.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A16" s="7" t="n">
         <v>19</v>
       </c>
       <c r="B16" s="7" t="s">
@@ -2551,13 +2273,13 @@
         <v>43</v>
       </c>
       <c r="E16" s="7" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="F16" s="7" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="G16" s="14" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="H16" s="7" t="s">
         <v>56</v>
@@ -2565,15 +2287,15 @@
       <c r="I16" s="7"/>
       <c r="J16" s="7"/>
       <c r="K16" s="7"/>
-      <c r="L16" s="7">
+      <c r="L16" s="7" t="n">
         <v>1</v>
       </c>
       <c r="M16" s="7"/>
       <c r="N16" s="7"/>
       <c r="O16" s="7" t="s">
-        <v>93</v>
-      </c>
-      <c r="P16" s="10">
+        <v>94</v>
+      </c>
+      <c r="P16" s="10" t="n">
         <v>4650075420409</v>
       </c>
       <c r="Q16" s="10"/>
@@ -2596,30 +2318,30 @@
       <c r="AB16" s="7"/>
       <c r="AC16" s="7"/>
       <c r="AD16" s="7" t="s">
-        <v>184</v>
+        <v>60</v>
       </c>
       <c r="AE16" s="7"/>
       <c r="AF16" s="7"/>
       <c r="AG16" s="7" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="AH16" s="9"/>
       <c r="AI16" s="7"/>
       <c r="AJ16" s="7"/>
       <c r="AK16" s="7"/>
-      <c r="AL16" s="7">
+      <c r="AL16" s="7" t="n">
         <v>4</v>
       </c>
-      <c r="AM16" s="7">
+      <c r="AM16" s="7" t="n">
         <v>14</v>
       </c>
       <c r="AN16" s="7"/>
-      <c r="AO16" s="7">
+      <c r="AO16" s="7" t="n">
         <v>15</v>
       </c>
     </row>
-    <row r="17" spans="1:41" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="7">
+    <row r="17" customFormat="false" ht="21.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A17" s="7" t="n">
         <v>15</v>
       </c>
       <c r="B17" s="7" t="s">
@@ -2632,13 +2354,13 @@
         <v>43</v>
       </c>
       <c r="E17" s="7" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="F17" s="7" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="G17" s="14" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="H17" s="7" t="s">
         <v>56</v>
@@ -2646,15 +2368,15 @@
       <c r="I17" s="7"/>
       <c r="J17" s="7"/>
       <c r="K17" s="7"/>
-      <c r="L17" s="7">
+      <c r="L17" s="7" t="n">
         <v>1</v>
       </c>
       <c r="M17" s="7"/>
       <c r="N17" s="7"/>
       <c r="O17" s="7" t="s">
-        <v>95</v>
-      </c>
-      <c r="P17" s="10">
+        <v>96</v>
+      </c>
+      <c r="P17" s="10" t="n">
         <v>4650075420508</v>
       </c>
       <c r="Q17" s="10"/>
@@ -2677,30 +2399,30 @@
       <c r="AB17" s="7"/>
       <c r="AC17" s="7"/>
       <c r="AD17" s="7" t="s">
-        <v>184</v>
+        <v>60</v>
       </c>
       <c r="AE17" s="7"/>
       <c r="AF17" s="7"/>
       <c r="AG17" s="7" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="AH17" s="9"/>
       <c r="AI17" s="7"/>
       <c r="AJ17" s="7"/>
       <c r="AK17" s="7"/>
-      <c r="AL17" s="7">
+      <c r="AL17" s="7" t="n">
         <v>4</v>
       </c>
-      <c r="AM17" s="7">
+      <c r="AM17" s="7" t="n">
         <v>16</v>
       </c>
       <c r="AN17" s="7"/>
-      <c r="AO17" s="13">
+      <c r="AO17" s="13" t="n">
         <v>15</v>
       </c>
     </row>
-    <row r="18" spans="1:41" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="7">
+    <row r="18" customFormat="false" ht="21.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A18" s="7" t="n">
         <v>20</v>
       </c>
       <c r="B18" s="7" t="s">
@@ -2713,13 +2435,13 @@
         <v>43</v>
       </c>
       <c r="E18" s="7" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="F18" s="7" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="G18" s="7" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="H18" s="7" t="s">
         <v>50</v>
@@ -2728,7 +2450,7 @@
         <v>44</v>
       </c>
       <c r="J18" s="12" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="K18" s="7"/>
       <c r="L18" s="7"/>
@@ -2761,25 +2483,25 @@
       <c r="AI18" s="7"/>
       <c r="AJ18" s="7"/>
       <c r="AK18" s="7"/>
-      <c r="AL18" s="7">
+      <c r="AL18" s="7" t="n">
         <v>2</v>
       </c>
-      <c r="AM18" s="7">
+      <c r="AM18" s="7" t="n">
         <v>20</v>
       </c>
       <c r="AN18" s="13" t="s">
-        <v>100</v>
-      </c>
-      <c r="AO18" s="7">
+        <v>101</v>
+      </c>
+      <c r="AO18" s="7" t="n">
         <v>300</v>
       </c>
     </row>
-    <row r="19" spans="1:41" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="7">
+    <row r="19" customFormat="false" ht="21.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A19" s="7" t="n">
         <v>72</v>
       </c>
       <c r="B19" s="7" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="C19" s="7" t="s">
         <v>42</v>
@@ -2788,13 +2510,13 @@
         <v>43</v>
       </c>
       <c r="E19" s="7" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="F19" s="7" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="G19" s="7" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="H19" s="7" t="s">
         <v>56</v>
@@ -2802,21 +2524,21 @@
       <c r="I19" s="7"/>
       <c r="J19" s="7"/>
       <c r="K19" s="7"/>
-      <c r="L19" s="16">
+      <c r="L19" s="16" t="n">
         <v>1</v>
       </c>
       <c r="M19" s="16"/>
       <c r="N19" s="16"/>
       <c r="O19" s="7" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="P19" s="10" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="Q19" s="10"/>
       <c r="R19" s="10"/>
       <c r="S19" s="10"/>
-      <c r="T19" s="17"/>
+      <c r="T19" s="0"/>
       <c r="U19" s="7" t="s">
         <v>57</v>
       </c>
@@ -2833,36 +2555,36 @@
       <c r="AB19" s="7"/>
       <c r="AC19" s="7"/>
       <c r="AD19" s="7" t="s">
-        <v>184</v>
+        <v>60</v>
       </c>
       <c r="AE19" s="7"/>
-      <c r="AF19" s="18"/>
-      <c r="AG19" s="19" t="s">
-        <v>60</v>
-      </c>
-      <c r="AH19" s="20">
-        <v>3.0317E-2</v>
+      <c r="AF19" s="17"/>
+      <c r="AG19" s="18" t="s">
+        <v>61</v>
+      </c>
+      <c r="AH19" s="19" t="n">
+        <v>0.030317</v>
       </c>
       <c r="AI19" s="7"/>
       <c r="AJ19" s="7"/>
       <c r="AK19" s="7"/>
-      <c r="AL19" s="7">
+      <c r="AL19" s="7" t="n">
         <v>3</v>
       </c>
-      <c r="AM19" s="7">
+      <c r="AM19" s="7" t="n">
         <v>767</v>
       </c>
       <c r="AN19" s="7"/>
-      <c r="AO19" s="7">
+      <c r="AO19" s="7" t="n">
         <v>20</v>
       </c>
     </row>
-    <row r="20" spans="1:41" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="7">
+    <row r="20" customFormat="false" ht="21.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A20" s="7" t="n">
         <v>66</v>
       </c>
       <c r="B20" s="7" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="C20" s="7" t="s">
         <v>42</v>
@@ -2871,13 +2593,13 @@
         <v>43</v>
       </c>
       <c r="E20" s="7" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="F20" s="7" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="G20" s="7" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="H20" s="7" t="s">
         <v>56</v>
@@ -2885,21 +2607,21 @@
       <c r="I20" s="7"/>
       <c r="J20" s="7"/>
       <c r="K20" s="7"/>
-      <c r="L20" s="16">
+      <c r="L20" s="16" t="n">
         <v>1</v>
       </c>
       <c r="M20" s="16"/>
       <c r="N20" s="16"/>
       <c r="O20" s="7" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="P20" s="10" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="Q20" s="10"/>
       <c r="R20" s="10"/>
       <c r="S20" s="10"/>
-      <c r="T20" s="17"/>
+      <c r="T20" s="0"/>
       <c r="U20" s="7" t="s">
         <v>57</v>
       </c>
@@ -2916,32 +2638,32 @@
       <c r="AB20" s="7"/>
       <c r="AC20" s="7"/>
       <c r="AD20" s="7" t="s">
-        <v>184</v>
+        <v>60</v>
       </c>
       <c r="AE20" s="7"/>
-      <c r="AF20" s="18"/>
-      <c r="AG20" s="19" t="s">
-        <v>60</v>
-      </c>
-      <c r="AH20" s="20">
-        <v>3.0317E-2</v>
+      <c r="AF20" s="17"/>
+      <c r="AG20" s="18" t="s">
+        <v>61</v>
+      </c>
+      <c r="AH20" s="19" t="n">
+        <v>0.030317</v>
       </c>
       <c r="AI20" s="7"/>
       <c r="AJ20" s="7"/>
       <c r="AK20" s="7"/>
-      <c r="AL20" s="7">
+      <c r="AL20" s="7" t="n">
         <v>3</v>
       </c>
-      <c r="AM20" s="7">
+      <c r="AM20" s="7" t="n">
         <v>759</v>
       </c>
       <c r="AN20" s="7"/>
-      <c r="AO20" s="7">
+      <c r="AO20" s="7" t="n">
         <v>20</v>
       </c>
     </row>
-    <row r="21" spans="1:41" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="7">
+    <row r="21" customFormat="false" ht="21.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A21" s="7" t="n">
         <v>42</v>
       </c>
       <c r="B21" s="7" t="s">
@@ -2955,10 +2677,10 @@
       </c>
       <c r="E21" s="7"/>
       <c r="F21" s="8" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="G21" s="8" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="H21" s="8" t="s">
         <v>43</v>
@@ -2992,19 +2714,19 @@
       <c r="AI21" s="7"/>
       <c r="AJ21" s="7"/>
       <c r="AK21" s="7"/>
-      <c r="AL21" s="10">
+      <c r="AL21" s="10" t="n">
         <v>1</v>
       </c>
-      <c r="AM21" s="10">
+      <c r="AM21" s="10" t="n">
         <v>310</v>
       </c>
       <c r="AN21" s="11" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="AO21" s="10"/>
     </row>
-    <row r="22" spans="1:41" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="7">
+    <row r="22" customFormat="false" ht="21.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A22" s="7" t="n">
         <v>43</v>
       </c>
       <c r="B22" s="7" t="s">
@@ -3018,10 +2740,10 @@
       </c>
       <c r="E22" s="7"/>
       <c r="F22" s="8" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="G22" s="8" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="H22" s="8" t="s">
         <v>43</v>
@@ -3055,21 +2777,21 @@
       <c r="AI22" s="7"/>
       <c r="AJ22" s="7"/>
       <c r="AK22" s="7"/>
-      <c r="AL22" s="10">
+      <c r="AL22" s="10" t="n">
         <v>1</v>
       </c>
-      <c r="AM22" s="10">
+      <c r="AM22" s="10" t="n">
         <v>312</v>
       </c>
-      <c r="AN22" s="7">
+      <c r="AN22" s="7" t="n">
         <v>33</v>
       </c>
-      <c r="AO22" s="10">
+      <c r="AO22" s="10" t="n">
         <v>310</v>
       </c>
     </row>
-    <row r="23" spans="1:41" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A23" s="7">
+    <row r="23" customFormat="false" ht="21.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A23" s="7" t="n">
         <v>34</v>
       </c>
       <c r="B23" s="7" t="s">
@@ -3079,24 +2801,24 @@
         <v>42</v>
       </c>
       <c r="D23" s="7" t="s">
-        <v>114</v>
-      </c>
-      <c r="E23" s="21" t="s">
         <v>115</v>
       </c>
-      <c r="F23" s="21" t="s">
+      <c r="E23" s="20" t="s">
         <v>116</v>
       </c>
+      <c r="F23" s="20" t="s">
+        <v>117</v>
+      </c>
       <c r="G23" s="7" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
       <c r="H23" s="7" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
       <c r="I23" s="7"/>
       <c r="J23" s="7"/>
       <c r="K23" s="7"/>
-      <c r="L23" s="7">
+      <c r="L23" s="7" t="n">
         <v>3</v>
       </c>
       <c r="M23" s="7"/>
@@ -3115,36 +2837,36 @@
       <c r="Z23" s="7"/>
       <c r="AA23" s="7"/>
       <c r="AB23" s="7" t="s">
-        <v>119</v>
+        <v>120</v>
       </c>
       <c r="AC23" s="7"/>
       <c r="AD23" s="7"/>
       <c r="AE23" s="7"/>
       <c r="AF23" s="7"/>
       <c r="AG23" s="15" t="s">
-        <v>60</v>
-      </c>
-      <c r="AH23" s="9">
-        <v>4.6667E-2</v>
+        <v>61</v>
+      </c>
+      <c r="AH23" s="9" t="n">
+        <v>0.046667</v>
       </c>
       <c r="AI23" s="7"/>
       <c r="AJ23" s="7"/>
       <c r="AK23" s="7"/>
-      <c r="AL23" s="7">
+      <c r="AL23" s="7" t="n">
         <v>2</v>
       </c>
-      <c r="AM23" s="7">
+      <c r="AM23" s="7" t="n">
         <v>33</v>
       </c>
       <c r="AN23" s="13" t="s">
-        <v>120</v>
-      </c>
-      <c r="AO23" s="7">
+        <v>121</v>
+      </c>
+      <c r="AO23" s="7" t="n">
         <v>312</v>
       </c>
     </row>
-    <row r="24" spans="1:41" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A24" s="7">
+    <row r="24" customFormat="false" ht="21.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A24" s="7" t="n">
         <v>35</v>
       </c>
       <c r="B24" s="7" t="s">
@@ -3154,24 +2876,24 @@
         <v>42</v>
       </c>
       <c r="D24" s="7" t="s">
-        <v>114</v>
-      </c>
-      <c r="E24" s="21" t="s">
         <v>115</v>
       </c>
-      <c r="F24" s="21" t="s">
-        <v>121</v>
+      <c r="E24" s="20" t="s">
+        <v>116</v>
+      </c>
+      <c r="F24" s="20" t="s">
+        <v>122</v>
       </c>
       <c r="G24" s="7" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="H24" s="7" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
       <c r="I24" s="7"/>
       <c r="J24" s="7"/>
       <c r="K24" s="7"/>
-      <c r="L24" s="7">
+      <c r="L24" s="7" t="n">
         <v>1</v>
       </c>
       <c r="M24" s="7"/>
@@ -3186,7 +2908,7 @@
         <v>57</v>
       </c>
       <c r="V24" s="7" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
       <c r="W24" s="7"/>
       <c r="X24" s="7"/>
@@ -3194,32 +2916,32 @@
       <c r="Z24" s="7"/>
       <c r="AA24" s="7"/>
       <c r="AB24" s="7"/>
-      <c r="AC24" s="22" t="s">
-        <v>185</v>
+      <c r="AC24" s="21" t="s">
+        <v>126</v>
       </c>
       <c r="AD24" s="7"/>
       <c r="AE24" s="7"/>
       <c r="AF24" s="7"/>
       <c r="AG24" s="15" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="AH24" s="9"/>
       <c r="AI24" s="7"/>
       <c r="AJ24" s="7"/>
       <c r="AK24" s="7"/>
-      <c r="AL24" s="7">
+      <c r="AL24" s="7" t="n">
         <v>3</v>
       </c>
-      <c r="AM24" s="7">
+      <c r="AM24" s="7" t="n">
         <v>34</v>
       </c>
       <c r="AN24" s="7"/>
-      <c r="AO24" s="7">
+      <c r="AO24" s="7" t="n">
         <v>33</v>
       </c>
     </row>
-    <row r="25" spans="1:41" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A25" s="7">
+    <row r="25" customFormat="false" ht="21.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A25" s="7" t="n">
         <v>36</v>
       </c>
       <c r="B25" s="7" t="s">
@@ -3229,33 +2951,33 @@
         <v>42</v>
       </c>
       <c r="D25" s="7" t="s">
-        <v>114</v>
-      </c>
-      <c r="E25" s="21" t="s">
         <v>115</v>
       </c>
-      <c r="F25" s="21" t="s">
-        <v>125</v>
+      <c r="E25" s="20" t="s">
+        <v>116</v>
+      </c>
+      <c r="F25" s="20" t="s">
+        <v>127</v>
       </c>
       <c r="G25" s="7" t="s">
-        <v>126</v>
+        <v>128</v>
       </c>
       <c r="H25" s="7" t="s">
-        <v>127</v>
+        <v>129</v>
       </c>
       <c r="I25" s="7"/>
       <c r="J25" s="7"/>
       <c r="K25" s="7"/>
-      <c r="L25" s="7">
+      <c r="L25" s="7" t="n">
         <v>1</v>
       </c>
       <c r="M25" s="7"/>
       <c r="N25" s="7"/>
       <c r="O25" s="7" t="s">
-        <v>128</v>
+        <v>130</v>
       </c>
       <c r="P25" s="7" t="s">
-        <v>129</v>
+        <v>131</v>
       </c>
       <c r="Q25" s="7"/>
       <c r="R25" s="7"/>
@@ -3265,7 +2987,7 @@
         <v>57</v>
       </c>
       <c r="V25" s="7" t="s">
-        <v>130</v>
+        <v>132</v>
       </c>
       <c r="W25" s="7"/>
       <c r="X25" s="7"/>
@@ -3273,34 +2995,34 @@
       <c r="Z25" s="7"/>
       <c r="AA25" s="7"/>
       <c r="AB25" s="7" t="s">
-        <v>119</v>
+        <v>120</v>
       </c>
       <c r="AC25" s="7"/>
       <c r="AD25" s="7"/>
       <c r="AE25" s="7"/>
       <c r="AF25" s="7"/>
       <c r="AG25" s="15" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="AH25" s="9"/>
       <c r="AI25" s="7"/>
       <c r="AJ25" s="7"/>
       <c r="AK25" s="7" t="s">
-        <v>131</v>
-      </c>
-      <c r="AL25" s="7">
+        <v>133</v>
+      </c>
+      <c r="AL25" s="7" t="n">
         <v>3</v>
       </c>
-      <c r="AM25" s="7">
+      <c r="AM25" s="7" t="n">
         <v>35</v>
       </c>
       <c r="AN25" s="7"/>
-      <c r="AO25" s="7">
+      <c r="AO25" s="7" t="n">
         <v>33</v>
       </c>
     </row>
-    <row r="26" spans="1:41" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A26" s="7">
+    <row r="26" customFormat="false" ht="21.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A26" s="7" t="n">
         <v>37</v>
       </c>
       <c r="B26" s="7" t="s">
@@ -3310,33 +3032,33 @@
         <v>42</v>
       </c>
       <c r="D26" s="7" t="s">
-        <v>114</v>
-      </c>
-      <c r="E26" s="21" t="s">
         <v>115</v>
       </c>
-      <c r="F26" s="21" t="s">
-        <v>132</v>
+      <c r="E26" s="20" t="s">
+        <v>116</v>
+      </c>
+      <c r="F26" s="20" t="s">
+        <v>134</v>
       </c>
       <c r="G26" s="7" t="s">
-        <v>133</v>
+        <v>135</v>
       </c>
       <c r="H26" s="7" t="s">
-        <v>134</v>
+        <v>136</v>
       </c>
       <c r="I26" s="7"/>
       <c r="J26" s="7"/>
       <c r="K26" s="7"/>
-      <c r="L26" s="7">
+      <c r="L26" s="7" t="n">
         <v>1</v>
       </c>
       <c r="M26" s="7"/>
       <c r="N26" s="7"/>
       <c r="O26" s="7" t="s">
-        <v>128</v>
+        <v>130</v>
       </c>
       <c r="P26" s="7" t="s">
-        <v>129</v>
+        <v>131</v>
       </c>
       <c r="Q26" s="7"/>
       <c r="R26" s="7"/>
@@ -3346,7 +3068,7 @@
         <v>57</v>
       </c>
       <c r="V26" s="7" t="s">
-        <v>130</v>
+        <v>132</v>
       </c>
       <c r="W26" s="7"/>
       <c r="X26" s="7"/>
@@ -3354,34 +3076,34 @@
       <c r="Z26" s="7"/>
       <c r="AA26" s="7"/>
       <c r="AB26" s="7" t="s">
-        <v>119</v>
+        <v>120</v>
       </c>
       <c r="AC26" s="7"/>
       <c r="AD26" s="7"/>
       <c r="AE26" s="7"/>
       <c r="AF26" s="7"/>
       <c r="AG26" s="15" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="AH26" s="9"/>
       <c r="AI26" s="7"/>
       <c r="AJ26" s="7"/>
       <c r="AK26" s="7" t="s">
-        <v>135</v>
-      </c>
-      <c r="AL26" s="7">
+        <v>137</v>
+      </c>
+      <c r="AL26" s="7" t="n">
         <v>3</v>
       </c>
-      <c r="AM26" s="7">
+      <c r="AM26" s="7" t="n">
         <v>36</v>
       </c>
       <c r="AN26" s="7"/>
-      <c r="AO26" s="7">
+      <c r="AO26" s="7" t="n">
         <v>33</v>
       </c>
     </row>
-    <row r="27" spans="1:41" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A27" s="7">
+    <row r="27" customFormat="false" ht="21.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A27" s="7" t="n">
         <v>44</v>
       </c>
       <c r="B27" s="7" t="s">
@@ -3395,10 +3117,10 @@
       </c>
       <c r="E27" s="7"/>
       <c r="F27" s="8" t="s">
-        <v>136</v>
+        <v>138</v>
       </c>
       <c r="G27" s="8" t="s">
-        <v>137</v>
+        <v>139</v>
       </c>
       <c r="H27" s="8" t="s">
         <v>43</v>
@@ -3432,19 +3154,19 @@
       <c r="AI27" s="7"/>
       <c r="AJ27" s="7"/>
       <c r="AK27" s="7"/>
-      <c r="AL27" s="10">
+      <c r="AL27" s="10" t="n">
         <v>1</v>
       </c>
-      <c r="AM27" s="10">
+      <c r="AM27" s="10" t="n">
         <v>400</v>
       </c>
       <c r="AN27" s="11" t="s">
-        <v>138</v>
+        <v>140</v>
       </c>
       <c r="AO27" s="10"/>
     </row>
-    <row r="28" spans="1:41" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A28" s="7">
+    <row r="28" customFormat="false" ht="21.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A28" s="7" t="n">
         <v>23</v>
       </c>
       <c r="B28" s="7" t="s">
@@ -3457,13 +3179,13 @@
         <v>43</v>
       </c>
       <c r="E28" s="7" t="s">
-        <v>139</v>
+        <v>141</v>
       </c>
       <c r="F28" s="7" t="s">
-        <v>140</v>
+        <v>142</v>
       </c>
       <c r="G28" s="7" t="s">
-        <v>141</v>
+        <v>143</v>
       </c>
       <c r="H28" s="7" t="s">
         <v>56</v>
@@ -3471,28 +3193,28 @@
       <c r="I28" s="7"/>
       <c r="J28" s="7"/>
       <c r="K28" s="7"/>
-      <c r="L28" s="7">
+      <c r="L28" s="7" t="n">
         <v>1</v>
       </c>
       <c r="M28" s="7"/>
       <c r="N28" s="7"/>
       <c r="O28" s="7" t="s">
-        <v>142</v>
+        <v>144</v>
       </c>
       <c r="P28" s="7" t="s">
-        <v>143</v>
+        <v>145</v>
       </c>
       <c r="Q28" s="7"/>
       <c r="R28" s="7"/>
       <c r="S28" s="7"/>
       <c r="T28" s="7" t="s">
-        <v>143</v>
+        <v>145</v>
       </c>
       <c r="U28" s="7" t="s">
         <v>57</v>
       </c>
       <c r="V28" s="7" t="s">
-        <v>144</v>
+        <v>146</v>
       </c>
       <c r="W28" s="7"/>
       <c r="X28" s="7"/>
@@ -3501,33 +3223,33 @@
       <c r="AA28" s="7"/>
       <c r="AB28" s="7"/>
       <c r="AC28" s="7" t="s">
-        <v>186</v>
+        <v>147</v>
       </c>
       <c r="AD28" s="7"/>
       <c r="AE28" s="7"/>
       <c r="AF28" s="7"/>
       <c r="AG28" s="7" t="s">
-        <v>60</v>
-      </c>
-      <c r="AH28" s="9">
-        <v>0.16666700000000001</v>
+        <v>61</v>
+      </c>
+      <c r="AH28" s="9" t="n">
+        <v>0.166667</v>
       </c>
       <c r="AI28" s="15"/>
-      <c r="AJ28" s="23"/>
+      <c r="AJ28" s="22"/>
       <c r="AK28" s="7"/>
-      <c r="AL28" s="7">
+      <c r="AL28" s="7" t="n">
         <v>2</v>
       </c>
-      <c r="AM28" s="7">
+      <c r="AM28" s="7" t="n">
         <v>22</v>
       </c>
       <c r="AN28" s="7"/>
-      <c r="AO28" s="7">
+      <c r="AO28" s="7" t="n">
         <v>400</v>
       </c>
     </row>
-    <row r="29" spans="1:41" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A29" s="7">
+    <row r="29" customFormat="false" ht="21.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A29" s="7" t="n">
         <v>24</v>
       </c>
       <c r="B29" s="7" t="s">
@@ -3540,21 +3262,21 @@
         <v>43</v>
       </c>
       <c r="E29" s="7" t="s">
-        <v>145</v>
+        <v>148</v>
       </c>
       <c r="F29" s="7" t="s">
-        <v>146</v>
+        <v>149</v>
       </c>
       <c r="G29" s="7" t="s">
-        <v>147</v>
+        <v>150</v>
       </c>
       <c r="H29" s="7" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
       <c r="I29" s="7"/>
       <c r="J29" s="7"/>
       <c r="K29" s="7"/>
-      <c r="L29" s="7">
+      <c r="L29" s="7" t="n">
         <v>1</v>
       </c>
       <c r="M29" s="7"/>
@@ -3576,35 +3298,35 @@
       <c r="AA29" s="7"/>
       <c r="AB29" s="7"/>
       <c r="AC29" s="7" t="s">
-        <v>187</v>
+        <v>151</v>
       </c>
       <c r="AD29" s="7"/>
       <c r="AE29" s="7"/>
       <c r="AF29" s="7"/>
       <c r="AG29" s="7" t="s">
-        <v>60</v>
-      </c>
-      <c r="AH29" s="9">
-        <v>0.20333300000000001</v>
+        <v>61</v>
+      </c>
+      <c r="AH29" s="9" t="n">
+        <v>0.203333</v>
       </c>
       <c r="AI29" s="15"/>
       <c r="AJ29" s="7"/>
       <c r="AK29" s="7"/>
-      <c r="AL29" s="7">
+      <c r="AL29" s="7" t="n">
         <v>2</v>
       </c>
-      <c r="AM29" s="7">
+      <c r="AM29" s="7" t="n">
         <v>23</v>
       </c>
-      <c r="AN29" s="7">
+      <c r="AN29" s="7" t="n">
         <v>856</v>
       </c>
-      <c r="AO29" s="7">
+      <c r="AO29" s="7" t="n">
         <v>400</v>
       </c>
     </row>
-    <row r="30" spans="1:41" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A30" s="7">
+    <row r="30" customFormat="false" ht="21.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A30" s="7" t="n">
         <v>25</v>
       </c>
       <c r="B30" s="7" t="s">
@@ -3617,13 +3339,13 @@
         <v>43</v>
       </c>
       <c r="E30" s="7" t="s">
-        <v>145</v>
+        <v>148</v>
       </c>
       <c r="F30" s="7" t="s">
-        <v>148</v>
+        <v>152</v>
       </c>
       <c r="G30" s="7" t="s">
-        <v>149</v>
+        <v>153</v>
       </c>
       <c r="H30" s="7" t="s">
         <v>56</v>
@@ -3631,61 +3353,61 @@
       <c r="I30" s="7"/>
       <c r="J30" s="7"/>
       <c r="K30" s="7"/>
-      <c r="L30" s="7">
+      <c r="L30" s="7" t="n">
         <v>3</v>
       </c>
       <c r="M30" s="7"/>
       <c r="N30" s="7"/>
-      <c r="O30" s="24" t="s">
-        <v>128</v>
-      </c>
-      <c r="P30" s="25" t="s">
-        <v>129</v>
+      <c r="O30" s="23" t="s">
+        <v>130</v>
+      </c>
+      <c r="P30" s="24" t="s">
+        <v>131</v>
       </c>
       <c r="Q30" s="7"/>
       <c r="R30" s="7"/>
       <c r="S30" s="7"/>
-      <c r="T30" s="26"/>
+      <c r="T30" s="25"/>
       <c r="U30" s="7" t="s">
         <v>57</v>
       </c>
-      <c r="V30" s="24" t="s">
-        <v>130</v>
+      <c r="V30" s="23" t="s">
+        <v>132</v>
       </c>
       <c r="W30" s="7"/>
       <c r="X30" s="7" t="s">
-        <v>150</v>
+        <v>154</v>
       </c>
       <c r="Y30" s="7"/>
       <c r="Z30" s="7"/>
       <c r="AA30" s="7"/>
       <c r="AB30" s="7"/>
       <c r="AC30" s="7" t="s">
-        <v>187</v>
+        <v>151</v>
       </c>
       <c r="AD30" s="7"/>
       <c r="AE30" s="7"/>
       <c r="AF30" s="7"/>
       <c r="AG30" s="7" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="AH30" s="9"/>
       <c r="AI30" s="15"/>
       <c r="AJ30" s="7"/>
       <c r="AK30" s="7"/>
-      <c r="AL30" s="7">
+      <c r="AL30" s="7" t="n">
         <v>3</v>
       </c>
-      <c r="AM30" s="7">
+      <c r="AM30" s="7" t="n">
         <v>856</v>
       </c>
       <c r="AN30" s="7"/>
-      <c r="AO30" s="7">
+      <c r="AO30" s="7" t="n">
         <v>23</v>
       </c>
     </row>
-    <row r="31" spans="1:41" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A31" s="7">
+    <row r="31" customFormat="false" ht="21.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A31" s="7" t="n">
         <v>26</v>
       </c>
       <c r="B31" s="7" t="s">
@@ -3698,21 +3420,21 @@
         <v>43</v>
       </c>
       <c r="E31" s="7" t="s">
-        <v>145</v>
+        <v>148</v>
       </c>
       <c r="F31" s="7" t="s">
-        <v>151</v>
+        <v>155</v>
       </c>
       <c r="G31" s="7" t="s">
-        <v>152</v>
+        <v>156</v>
       </c>
       <c r="H31" s="7" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
       <c r="I31" s="7"/>
       <c r="J31" s="7"/>
       <c r="K31" s="7"/>
-      <c r="L31" s="7">
+      <c r="L31" s="7" t="n">
         <v>1</v>
       </c>
       <c r="M31" s="7"/>
@@ -3734,35 +3456,35 @@
       <c r="AA31" s="7"/>
       <c r="AB31" s="7"/>
       <c r="AC31" s="7" t="s">
-        <v>188</v>
+        <v>157</v>
       </c>
       <c r="AD31" s="7"/>
       <c r="AE31" s="7"/>
       <c r="AF31" s="7"/>
       <c r="AG31" s="7" t="s">
-        <v>60</v>
-      </c>
-      <c r="AH31" s="9">
-        <v>8.3333000000000004E-2</v>
+        <v>61</v>
+      </c>
+      <c r="AH31" s="9" t="n">
+        <v>0.083333</v>
       </c>
       <c r="AI31" s="15"/>
       <c r="AJ31" s="7"/>
       <c r="AK31" s="7"/>
-      <c r="AL31" s="7">
+      <c r="AL31" s="7" t="n">
         <v>2</v>
       </c>
-      <c r="AM31" s="7">
+      <c r="AM31" s="7" t="n">
         <v>25</v>
       </c>
       <c r="AN31" s="13" t="s">
-        <v>153</v>
-      </c>
-      <c r="AO31" s="7">
+        <v>158</v>
+      </c>
+      <c r="AO31" s="7" t="n">
         <v>400</v>
       </c>
     </row>
-    <row r="32" spans="1:41" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A32" s="7">
+    <row r="32" customFormat="false" ht="21.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A32" s="7" t="n">
         <v>27</v>
       </c>
       <c r="B32" s="7" t="s">
@@ -3775,13 +3497,13 @@
         <v>43</v>
       </c>
       <c r="E32" s="7" t="s">
-        <v>145</v>
+        <v>148</v>
       </c>
       <c r="F32" s="7" t="s">
-        <v>154</v>
+        <v>159</v>
       </c>
       <c r="G32" s="7" t="s">
-        <v>155</v>
+        <v>160</v>
       </c>
       <c r="H32" s="7" t="s">
         <v>56</v>
@@ -3789,19 +3511,19 @@
       <c r="I32" s="7"/>
       <c r="J32" s="7"/>
       <c r="K32" s="7"/>
-      <c r="L32" s="7">
+      <c r="L32" s="7" t="n">
         <v>1</v>
       </c>
       <c r="M32" s="7"/>
       <c r="N32" s="7"/>
       <c r="O32" s="7" t="s">
-        <v>156</v>
+        <v>161</v>
       </c>
       <c r="P32" s="7" t="s">
-        <v>156</v>
+        <v>161</v>
       </c>
       <c r="Q32" s="7" t="s">
-        <v>156</v>
+        <v>161</v>
       </c>
       <c r="R32" s="7"/>
       <c r="S32" s="7"/>
@@ -3810,7 +3532,7 @@
         <v>57</v>
       </c>
       <c r="V32" s="7" t="s">
-        <v>157</v>
+        <v>162</v>
       </c>
       <c r="W32" s="7"/>
       <c r="X32" s="7"/>
@@ -3819,31 +3541,31 @@
       <c r="AA32" s="7"/>
       <c r="AB32" s="7"/>
       <c r="AC32" s="7" t="s">
-        <v>188</v>
+        <v>157</v>
       </c>
       <c r="AD32" s="7"/>
       <c r="AE32" s="7"/>
       <c r="AF32" s="7"/>
       <c r="AG32" s="7" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="AH32" s="9"/>
       <c r="AI32" s="15"/>
       <c r="AJ32" s="7"/>
       <c r="AK32" s="7"/>
-      <c r="AL32" s="7">
+      <c r="AL32" s="7" t="n">
         <v>3</v>
       </c>
-      <c r="AM32" s="7">
+      <c r="AM32" s="7" t="n">
         <v>26</v>
       </c>
       <c r="AN32" s="7"/>
-      <c r="AO32" s="7">
+      <c r="AO32" s="7" t="n">
         <v>25</v>
       </c>
     </row>
-    <row r="33" spans="1:41" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A33" s="7">
+    <row r="33" customFormat="false" ht="21.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A33" s="7" t="n">
         <v>38</v>
       </c>
       <c r="B33" s="7" t="s">
@@ -3853,24 +3575,24 @@
         <v>42</v>
       </c>
       <c r="D33" s="7" t="s">
-        <v>158</v>
-      </c>
-      <c r="E33" s="21" t="s">
-        <v>115</v>
-      </c>
-      <c r="F33" s="21" t="s">
-        <v>159</v>
-      </c>
-      <c r="G33" s="21" t="s">
-        <v>160</v>
+        <v>163</v>
+      </c>
+      <c r="E33" s="20" t="s">
+        <v>116</v>
+      </c>
+      <c r="F33" s="20" t="s">
+        <v>164</v>
+      </c>
+      <c r="G33" s="20" t="s">
+        <v>165</v>
       </c>
       <c r="H33" s="7" t="s">
-        <v>161</v>
+        <v>166</v>
       </c>
       <c r="I33" s="7"/>
       <c r="J33" s="7"/>
       <c r="K33" s="7" t="s">
-        <v>162</v>
+        <v>167</v>
       </c>
       <c r="L33" s="7"/>
       <c r="M33" s="7"/>
@@ -3883,7 +3605,7 @@
       <c r="T33" s="7"/>
       <c r="U33" s="7"/>
       <c r="V33" s="7" t="s">
-        <v>163</v>
+        <v>168</v>
       </c>
       <c r="W33" s="7"/>
       <c r="X33" s="7"/>
@@ -3901,16 +3623,16 @@
       <c r="AJ33" s="7"/>
       <c r="AK33" s="7"/>
       <c r="AL33" s="7"/>
-      <c r="AM33" s="7">
+      <c r="AM33" s="7" t="n">
         <v>38</v>
       </c>
       <c r="AN33" s="13" t="s">
-        <v>164</v>
+        <v>169</v>
       </c>
       <c r="AO33" s="7"/>
     </row>
-    <row r="34" spans="1:41" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A34" s="7">
+    <row r="34" customFormat="false" ht="21.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A34" s="7" t="n">
         <v>39</v>
       </c>
       <c r="B34" s="7" t="s">
@@ -3920,31 +3642,31 @@
         <v>42</v>
       </c>
       <c r="D34" s="7" t="s">
-        <v>158</v>
-      </c>
-      <c r="E34" s="21" t="s">
-        <v>139</v>
-      </c>
-      <c r="F34" s="21" t="s">
-        <v>165</v>
-      </c>
-      <c r="G34" s="21" t="s">
-        <v>166</v>
+        <v>163</v>
+      </c>
+      <c r="E34" s="20" t="s">
+        <v>141</v>
+      </c>
+      <c r="F34" s="20" t="s">
+        <v>170</v>
+      </c>
+      <c r="G34" s="20" t="s">
+        <v>171</v>
       </c>
       <c r="H34" s="7" t="s">
-        <v>167</v>
+        <v>172</v>
       </c>
       <c r="I34" s="7"/>
       <c r="J34" s="7"/>
       <c r="K34" s="7" t="s">
-        <v>168</v>
+        <v>173</v>
       </c>
       <c r="L34" s="7"/>
       <c r="M34" s="7"/>
       <c r="N34" s="7"/>
       <c r="O34" s="7"/>
       <c r="P34" s="13" t="s">
-        <v>169</v>
+        <v>174</v>
       </c>
       <c r="Q34" s="7"/>
       <c r="R34" s="7"/>
@@ -3952,7 +3674,7 @@
       <c r="T34" s="7"/>
       <c r="U34" s="7"/>
       <c r="V34" s="7" t="s">
-        <v>163</v>
+        <v>168</v>
       </c>
       <c r="W34" s="7"/>
       <c r="X34" s="7"/>
@@ -3970,16 +3692,16 @@
       <c r="AJ34" s="7"/>
       <c r="AK34" s="7"/>
       <c r="AL34" s="7"/>
-      <c r="AM34" s="7">
+      <c r="AM34" s="7" t="n">
         <v>39</v>
       </c>
-      <c r="AN34" s="7">
+      <c r="AN34" s="7" t="n">
         <v>22</v>
       </c>
       <c r="AO34" s="7"/>
     </row>
-    <row r="35" spans="1:41" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A35" s="7">
+    <row r="35" customFormat="false" ht="21.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A35" s="7" t="n">
         <v>40</v>
       </c>
       <c r="B35" s="7" t="s">
@@ -3989,31 +3711,31 @@
         <v>42</v>
       </c>
       <c r="D35" s="7" t="s">
-        <v>158</v>
+        <v>163</v>
       </c>
       <c r="E35" s="7" t="s">
-        <v>145</v>
+        <v>148</v>
       </c>
       <c r="F35" s="7" t="s">
-        <v>170</v>
+        <v>175</v>
       </c>
       <c r="G35" s="7" t="s">
-        <v>171</v>
+        <v>176</v>
       </c>
       <c r="H35" s="7" t="s">
-        <v>167</v>
+        <v>172</v>
       </c>
       <c r="I35" s="7"/>
       <c r="J35" s="7"/>
       <c r="K35" s="7" t="s">
-        <v>168</v>
+        <v>173</v>
       </c>
       <c r="L35" s="7"/>
       <c r="M35" s="7"/>
       <c r="N35" s="7"/>
       <c r="O35" s="7"/>
       <c r="P35" s="13" t="s">
-        <v>172</v>
+        <v>177</v>
       </c>
       <c r="Q35" s="7"/>
       <c r="R35" s="7"/>
@@ -4021,7 +3743,7 @@
       <c r="T35" s="7"/>
       <c r="U35" s="7"/>
       <c r="V35" s="7" t="s">
-        <v>163</v>
+        <v>168</v>
       </c>
       <c r="W35" s="7"/>
       <c r="X35" s="7"/>
@@ -4039,16 +3761,16 @@
       <c r="AJ35" s="7"/>
       <c r="AK35" s="7"/>
       <c r="AL35" s="7"/>
-      <c r="AM35" s="7">
+      <c r="AM35" s="7" t="n">
         <v>40</v>
       </c>
-      <c r="AN35" s="7">
+      <c r="AN35" s="7" t="n">
         <v>23</v>
       </c>
       <c r="AO35" s="7"/>
     </row>
-    <row r="36" spans="1:41" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A36" s="7">
+    <row r="36" customFormat="false" ht="21.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A36" s="7" t="n">
         <v>41</v>
       </c>
       <c r="B36" s="7" t="s">
@@ -4058,31 +3780,31 @@
         <v>42</v>
       </c>
       <c r="D36" s="7" t="s">
-        <v>158</v>
+        <v>163</v>
       </c>
       <c r="E36" s="7" t="s">
-        <v>145</v>
+        <v>148</v>
       </c>
       <c r="F36" s="7" t="s">
-        <v>170</v>
+        <v>175</v>
       </c>
       <c r="G36" s="7" t="s">
-        <v>171</v>
+        <v>176</v>
       </c>
       <c r="H36" s="7" t="s">
-        <v>167</v>
+        <v>172</v>
       </c>
       <c r="I36" s="7"/>
       <c r="J36" s="7"/>
       <c r="K36" s="7" t="s">
-        <v>168</v>
+        <v>173</v>
       </c>
       <c r="L36" s="7"/>
       <c r="M36" s="7"/>
       <c r="N36" s="7"/>
       <c r="O36" s="7"/>
       <c r="P36" s="13" t="s">
-        <v>173</v>
+        <v>178</v>
       </c>
       <c r="Q36" s="7"/>
       <c r="R36" s="7"/>
@@ -4090,7 +3812,7 @@
       <c r="T36" s="7"/>
       <c r="U36" s="7"/>
       <c r="V36" s="7" t="s">
-        <v>163</v>
+        <v>168</v>
       </c>
       <c r="W36" s="7"/>
       <c r="X36" s="7"/>
@@ -4108,16 +3830,16 @@
       <c r="AJ36" s="7"/>
       <c r="AK36" s="7"/>
       <c r="AL36" s="7"/>
-      <c r="AM36" s="7">
+      <c r="AM36" s="7" t="n">
         <v>41</v>
       </c>
-      <c r="AN36" s="7">
+      <c r="AN36" s="7" t="n">
         <v>25</v>
       </c>
       <c r="AO36" s="7"/>
     </row>
-    <row r="37" spans="1:41" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A37" s="7">
+    <row r="37" customFormat="false" ht="21.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A37" s="7" t="n">
         <v>43</v>
       </c>
       <c r="B37" s="7" t="s">
@@ -4127,33 +3849,33 @@
         <v>42</v>
       </c>
       <c r="D37" s="7" t="s">
-        <v>158</v>
+        <v>163</v>
       </c>
       <c r="E37" s="7" t="s">
-        <v>174</v>
-      </c>
-      <c r="F37" s="21" t="s">
-        <v>175</v>
-      </c>
-      <c r="G37" s="21" t="s">
-        <v>176</v>
+        <v>179</v>
+      </c>
+      <c r="F37" s="20" t="s">
+        <v>180</v>
+      </c>
+      <c r="G37" s="20" t="s">
+        <v>181</v>
       </c>
       <c r="H37" s="7" t="s">
-        <v>167</v>
+        <v>172</v>
       </c>
       <c r="I37" s="7"/>
       <c r="J37" s="7"/>
       <c r="K37" s="7" t="s">
-        <v>168</v>
+        <v>173</v>
       </c>
       <c r="L37" s="7"/>
       <c r="M37" s="7"/>
       <c r="N37" s="7"/>
       <c r="O37" s="7" t="s">
-        <v>177</v>
+        <v>182</v>
       </c>
       <c r="P37" s="13" t="s">
-        <v>178</v>
+        <v>183</v>
       </c>
       <c r="Q37" s="7"/>
       <c r="R37" s="7"/>
@@ -4161,7 +3883,7 @@
       <c r="T37" s="7"/>
       <c r="U37" s="7"/>
       <c r="V37" s="7" t="s">
-        <v>163</v>
+        <v>168</v>
       </c>
       <c r="W37" s="7"/>
       <c r="X37" s="7"/>
@@ -4179,16 +3901,16 @@
       <c r="AJ37" s="7"/>
       <c r="AK37" s="7"/>
       <c r="AL37" s="7"/>
-      <c r="AM37" s="7">
+      <c r="AM37" s="7" t="n">
         <v>44</v>
       </c>
       <c r="AN37" s="13" t="s">
-        <v>179</v>
+        <v>184</v>
       </c>
       <c r="AO37" s="7"/>
     </row>
-    <row r="38" spans="1:41" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A38" s="7">
+    <row r="38" customFormat="false" ht="21.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A38" s="7" t="n">
         <v>44</v>
       </c>
       <c r="B38" s="7" t="s">
@@ -4198,33 +3920,33 @@
         <v>42</v>
       </c>
       <c r="D38" s="7" t="s">
-        <v>158</v>
+        <v>163</v>
       </c>
       <c r="E38" s="7" t="s">
-        <v>174</v>
-      </c>
-      <c r="F38" s="21" t="s">
-        <v>175</v>
-      </c>
-      <c r="G38" s="21" t="s">
-        <v>176</v>
+        <v>179</v>
+      </c>
+      <c r="F38" s="20" t="s">
+        <v>180</v>
+      </c>
+      <c r="G38" s="20" t="s">
+        <v>181</v>
       </c>
       <c r="H38" s="7" t="s">
-        <v>167</v>
+        <v>172</v>
       </c>
       <c r="I38" s="7"/>
       <c r="J38" s="7"/>
       <c r="K38" s="7" t="s">
-        <v>168</v>
+        <v>173</v>
       </c>
       <c r="L38" s="7"/>
       <c r="M38" s="7"/>
       <c r="N38" s="7"/>
       <c r="O38" s="7" t="s">
-        <v>177</v>
+        <v>182</v>
       </c>
       <c r="P38" s="13" t="s">
-        <v>180</v>
+        <v>185</v>
       </c>
       <c r="Q38" s="7"/>
       <c r="R38" s="7"/>
@@ -4232,7 +3954,7 @@
       <c r="T38" s="7"/>
       <c r="U38" s="7"/>
       <c r="V38" s="7" t="s">
-        <v>163</v>
+        <v>168</v>
       </c>
       <c r="W38" s="7"/>
       <c r="X38" s="7"/>
@@ -4250,16 +3972,16 @@
       <c r="AJ38" s="7"/>
       <c r="AK38" s="7"/>
       <c r="AL38" s="7"/>
-      <c r="AM38" s="7">
+      <c r="AM38" s="7" t="n">
         <v>45</v>
       </c>
       <c r="AN38" s="13" t="s">
-        <v>164</v>
+        <v>169</v>
       </c>
       <c r="AO38" s="7"/>
     </row>
-    <row r="39" spans="1:41" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A39" s="7">
+    <row r="39" customFormat="false" ht="21.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A39" s="7" t="n">
         <v>904</v>
       </c>
       <c r="B39" s="7" t="s">
@@ -4269,35 +3991,35 @@
         <v>42</v>
       </c>
       <c r="D39" s="7" t="s">
-        <v>158</v>
-      </c>
-      <c r="E39" s="21"/>
-      <c r="F39" s="21" t="s">
-        <v>181</v>
-      </c>
-      <c r="G39" s="21" t="s">
-        <v>182</v>
+        <v>163</v>
+      </c>
+      <c r="E39" s="20"/>
+      <c r="F39" s="20" t="s">
+        <v>186</v>
+      </c>
+      <c r="G39" s="20" t="s">
+        <v>187</v>
       </c>
       <c r="H39" s="7" t="s">
-        <v>182</v>
+        <v>187</v>
       </c>
       <c r="I39" s="7"/>
       <c r="J39" s="7"/>
       <c r="K39" s="7" t="s">
-        <v>183</v>
+        <v>188</v>
       </c>
       <c r="L39" s="16"/>
       <c r="M39" s="16"/>
       <c r="N39" s="16"/>
       <c r="O39" s="7"/>
-      <c r="P39" s="27"/>
+      <c r="P39" s="26"/>
       <c r="Q39" s="7"/>
       <c r="R39" s="7"/>
       <c r="S39" s="7"/>
       <c r="T39" s="7"/>
       <c r="U39" s="7"/>
       <c r="V39" s="7" t="s">
-        <v>163</v>
+        <v>168</v>
       </c>
       <c r="W39" s="7"/>
       <c r="X39" s="7"/>
@@ -4308,22 +4030,28 @@
       <c r="AC39" s="7"/>
       <c r="AD39" s="7"/>
       <c r="AE39" s="7"/>
-      <c r="AF39" s="20"/>
+      <c r="AF39" s="19"/>
       <c r="AG39" s="7"/>
       <c r="AH39" s="7"/>
       <c r="AI39" s="7"/>
       <c r="AJ39" s="7"/>
       <c r="AK39" s="7"/>
       <c r="AL39" s="7"/>
-      <c r="AM39" s="7">
+      <c r="AM39" s="7" t="n">
         <v>904</v>
       </c>
       <c r="AN39" s="7"/>
       <c r="AO39" s="7"/>
     </row>
   </sheetData>
-  <autoFilter ref="A1:AO39" xr:uid="{00000000-0009-0000-0000-000000000000}"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
-  <pageSetup paperSize="0" scale="0" firstPageNumber="0" orientation="portrait" usePrinterDefaults="0" horizontalDpi="0" verticalDpi="0" copies="0"/>
+  <autoFilter ref="A1:AO39"/>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader/>
+    <oddFooter/>
+  </headerFooter>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>